<commit_message>
already the right formula
</commit_message>
<xml_diff>
--- a/bigdata/GPUs and hashrate.xlsx
+++ b/bigdata/GPUs and hashrate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ColorKat\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC5DCD0-E09D-4B92-968B-E77B8C91E777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1EE246-F732-4D40-A75D-97B62177C7DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="570" windowWidth="29040" windowHeight="15750" xr2:uid="{9B139ECC-C724-4273-A99C-4A05415BDC43}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="240">
   <si>
     <t>Memory</t>
   </si>
@@ -129,9 +129,6 @@
     <t>700 watt</t>
   </si>
   <si>
-    <t>Производительность</t>
-  </si>
-  <si>
     <t>75W</t>
   </si>
   <si>
@@ -423,9 +420,6 @@
     <t>Cuda+count</t>
   </si>
   <si>
-    <t>Hash+Rate</t>
-  </si>
-  <si>
     <t>RTX3070Ti</t>
   </si>
   <si>
@@ -726,18 +720,12 @@
     <t>Bit ^3</t>
   </si>
   <si>
-    <t>cuda*2</t>
-  </si>
-  <si>
     <t>GTX1060</t>
   </si>
   <si>
     <t>bandwidth</t>
   </si>
   <si>
-    <t>40% -&gt; 80%</t>
-  </si>
-  <si>
     <t>*2</t>
   </si>
   <si>
@@ -748,13 +736,31 @@
   </si>
   <si>
     <t>5888/6.4 * 448*2 / 13360 = 61.7 ----------- 6144/6.4 * 608*2 / 13360 = 87.3 -------- 2560/6.4 * 448*2 / 13360 = 27</t>
+  </si>
+  <si>
+    <t>Уточненный hashrate</t>
+  </si>
+  <si>
+    <t>Hashrate</t>
+  </si>
+  <si>
+    <t>cuda</t>
+  </si>
+  <si>
+    <t>17Mh/s</t>
+  </si>
+  <si>
+    <t>56Mh/s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,8 +839,92 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -868,6 +958,21 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE9ECEF"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1072,11 +1177,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1155,23 +1264,8 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1179,11 +1273,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1197,14 +1297,56 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="19" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Вывод" xfId="1" builtinId="21"/>
+    <cellStyle name="Нейтральный" xfId="5" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="4" builtinId="27"/>
+    <cellStyle name="Финансовый" xfId="2" builtinId="3"/>
+    <cellStyle name="Хороший" xfId="3" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1275,6 +1417,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1586,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21026847-03F0-4510-944F-5EFA55B75642}">
   <dimension ref="A1:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,71 +1745,71 @@
     <col min="6" max="6" width="25.28515625" style="28" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="28" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" style="55" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" customWidth="1"/>
     <col min="14" max="14" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="44" t="s">
+      <c r="D1" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="E1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="45" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>130</v>
+        <v>236</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>203</v>
+        <v>235</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>201</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
@@ -1674,41 +1819,41 @@
       <c r="T2" s="15"/>
       <c r="U2" s="9"/>
     </row>
-    <row r="3" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="F3" s="24" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="F3" s="45" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="29"/>
-      <c r="J3" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="M3" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="N3" s="30" t="s">
-        <v>96</v>
+      <c r="J3" s="56" t="s">
+        <v>202</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>95</v>
       </c>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
       <c r="T3" s="16"/>
       <c r="U3" s="10"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="2">
         <v>2560</v>
@@ -1719,7 +1864,7 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="48">
         <v>128</v>
       </c>
       <c r="F4" s="27">
@@ -1729,25 +1874,29 @@
         <v>1780</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I4" t="e">
         <f>B</f>
         <v>#NAME?</v>
       </c>
-      <c r="M4" s="37"/>
-      <c r="N4" s="31"/>
+      <c r="J4" s="55">
+        <f t="shared" ref="J4:J23" si="0">КОРЕНЬ(B4) *  КОРЕНЬ(E4) * (КОРЕНЬ(F4) + 1) / 2000 * 4,2</f>
+        <v>19.193647355292651</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="34"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
       <c r="T4" s="17"/>
       <c r="U4" s="9"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2">
         <v>3584</v>
@@ -1768,18 +1917,22 @@
         <v>1780</v>
       </c>
       <c r="H5" s="29" t="str">
-        <f>VLOOKUP(A5,M:N,2,0)</f>
+        <f>ВПР(A5;M:N;2;0)</f>
         <v>40-50MH/s*</v>
       </c>
-      <c r="M5" s="36" t="s">
-        <v>232</v>
+      <c r="J5" s="55">
+        <f t="shared" si="0"/>
+        <v>35.878564815611796</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>229</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O5" s="16"/>
       <c r="P5" s="16"/>
-      <c r="Q5" s="30"/>
+      <c r="Q5" s="33"/>
       <c r="R5" s="16"/>
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
@@ -1787,9 +1940,9 @@
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="2">
+        <v>67</v>
+      </c>
+      <c r="B6" s="51">
         <v>4864</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1798,7 +1951,7 @@
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="54">
         <v>256</v>
       </c>
       <c r="F6" s="27">
@@ -1808,19 +1961,23 @@
         <v>1670</v>
       </c>
       <c r="H6" s="29" t="str">
-        <f>VLOOKUP(A6,M:N,2,0)</f>
+        <f>ВПР(A6;M:N;2;0)</f>
         <v>55-63Mh/s</v>
       </c>
       <c r="I6">
         <v>60.2</v>
       </c>
-      <c r="M6" s="37"/>
+      <c r="J6" s="55">
+        <f t="shared" si="0"/>
+        <v>51.942589279207631</v>
+      </c>
+      <c r="M6" s="32"/>
       <c r="N6" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="31"/>
+      <c r="Q6" s="34"/>
       <c r="R6" s="17"/>
       <c r="S6" s="17"/>
       <c r="T6" s="17"/>
@@ -1828,9 +1985,9 @@
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="2">
+        <v>70</v>
+      </c>
+      <c r="B7" s="51">
         <v>5888</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1839,34 +1996,38 @@
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="54">
         <v>256</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="49">
         <v>448</v>
       </c>
       <c r="G7" s="2">
         <v>1770</v>
       </c>
       <c r="H7" s="29" t="str">
-        <f t="shared" ref="H7:H47" si="0">VLOOKUP(A7,M:N,2,0)</f>
+        <f t="shared" ref="H7:H47" si="1">ВПР(A7;M:N;2;0)</f>
         <v>55-63MH/s</v>
       </c>
       <c r="I7">
         <v>61.7</v>
       </c>
-      <c r="J7" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="M7" s="36" t="s">
+      <c r="J7" s="55">
+        <f t="shared" si="0"/>
+        <v>57.14927331289821</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="N7" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
       <c r="R7" s="16"/>
       <c r="S7" s="16"/>
       <c r="T7" s="16"/>
@@ -1874,7 +2035,7 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" s="2">
         <v>6144</v>
@@ -1885,33 +2046,37 @@
       <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="54">
         <v>256</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="49">
         <v>608</v>
       </c>
       <c r="G8" s="2">
         <v>1730</v>
       </c>
       <c r="H8" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80Mh/s*</v>
       </c>
       <c r="I8">
         <v>81.8</v>
       </c>
-      <c r="J8" s="28" t="s">
-        <v>231</v>
+      <c r="J8" s="55">
+        <f t="shared" si="0"/>
+        <v>67.574347249865355</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>237</v>
       </c>
       <c r="L8" t="s">
-        <v>237</v>
-      </c>
-      <c r="M8" s="37"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
+        <v>233</v>
+      </c>
+      <c r="M8" s="32"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17"/>
@@ -1919,7 +2084,7 @@
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>8704</v>
@@ -1940,35 +2105,36 @@
         <v>1710</v>
       </c>
       <c r="H9" s="29" t="str">
-        <f>VLOOKUP(A9,M:N,2,0)</f>
+        <f>ВПР(A9;M:N;2;0)</f>
         <v>95-105Mh/s</v>
       </c>
-      <c r="J9" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>234</v>
+      <c r="J9" s="55">
+        <f t="shared" si="0"/>
+        <v>100.12327447520398</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>230</v>
       </c>
       <c r="L9" t="s">
-        <v>235</v>
-      </c>
-      <c r="M9" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="M9" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>38</v>
       </c>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
-      <c r="R9" s="30"/>
+      <c r="R9" s="33"/>
       <c r="S9" s="16"/>
       <c r="T9" s="16"/>
       <c r="U9" s="10"/>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="2">
         <v>10240</v>
@@ -1982,31 +2148,38 @@
       <c r="E10" s="25">
         <v>384</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="49">
         <v>912</v>
       </c>
       <c r="G10" s="2">
         <v>1670</v>
       </c>
       <c r="H10" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>112Mh/s*</v>
+      </c>
+      <c r="I10">
+        <v>112</v>
+      </c>
+      <c r="J10" s="55">
         <f t="shared" si="0"/>
-        <v>112Mh/s*</v>
-      </c>
-      <c r="M10" s="37"/>
+        <v>129.92127104830539</v>
+      </c>
+      <c r="M10" s="32"/>
       <c r="N10" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
-      <c r="R10" s="31"/>
+      <c r="R10" s="34"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="9"/>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="2">
         <v>10496</v>
@@ -2020,33 +2193,40 @@
       <c r="E11" s="25">
         <v>384</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="49">
         <v>936</v>
       </c>
       <c r="G11" s="2">
         <v>1700</v>
       </c>
       <c r="H11" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>100-122Mh/s</v>
+      </c>
+      <c r="I11">
+        <v>121</v>
+      </c>
+      <c r="J11" s="55">
         <f t="shared" si="0"/>
-        <v>100-122Mh/s</v>
-      </c>
-      <c r="M11" s="36" t="s">
-        <v>104</v>
+        <v>133.19963696162753</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="34"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="35"/>
       <c r="U11" s="10"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B12" s="5">
         <v>2048</v>
@@ -2057,7 +2237,7 @@
       <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="48">
         <v>256</v>
       </c>
       <c r="F12" s="27">
@@ -2067,31 +2247,35 @@
         <v>1244</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="M12" s="37"/>
+        <v>64</v>
+      </c>
+      <c r="J12" s="55">
+        <f t="shared" si="0"/>
+        <v>24.278256899516737</v>
+      </c>
+      <c r="M12" s="32"/>
       <c r="N12" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="23"/>
       <c r="R12" s="23"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="35"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="36"/>
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="24" t="s">
@@ -2104,14 +2288,18 @@
         <v>11</v>
       </c>
       <c r="H13" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J13" s="55" t="e">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M13" s="36" t="s">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M13" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>106</v>
       </c>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
@@ -2123,13 +2311,13 @@
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="24" t="s">
         <v>6</v>
       </c>
@@ -2140,12 +2328,16 @@
         <v>10</v>
       </c>
       <c r="H14" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J14" s="55" t="e">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M14" s="37"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M14" s="32"/>
       <c r="N14" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
@@ -2160,8 +2352,8 @@
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="24" t="s">
         <v>7</v>
       </c>
@@ -2170,26 +2362,30 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J15" s="55" t="e">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M15" s="36" t="s">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M15" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="N15" s="16" t="s">
-        <v>45</v>
-      </c>
       <c r="O15" s="16"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="34"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="35"/>
       <c r="U15" s="10"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="2">
         <v>1920</v>
@@ -2210,26 +2406,30 @@
         <v>1680</v>
       </c>
       <c r="H16" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>25-30Mh/s</v>
+      </c>
+      <c r="J16" s="55">
         <f t="shared" si="0"/>
-        <v>25-30Mh/s</v>
-      </c>
-      <c r="M16" s="37"/>
+        <v>24.646722768834216</v>
+      </c>
+      <c r="M16" s="32"/>
       <c r="N16" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O16" s="17"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="35"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="36"/>
       <c r="U16" s="9"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="2">
+        <v>108</v>
+      </c>
+      <c r="B17" s="51">
         <v>2176</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -2238,7 +2438,7 @@
       <c r="D17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="54">
         <v>256</v>
       </c>
       <c r="F17" s="27">
@@ -2248,21 +2448,25 @@
         <v>1650</v>
       </c>
       <c r="H17" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 36-42 Mh/s</v>
       </c>
       <c r="I17">
         <v>38.700000000000003</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="J17" s="55">
+        <f t="shared" si="0"/>
+        <v>34.742115302946893</v>
+      </c>
+      <c r="M17" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="N17" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
-      <c r="Q17" s="30"/>
+      <c r="Q17" s="33"/>
       <c r="R17" s="16"/>
       <c r="S17" s="16"/>
       <c r="T17" s="16"/>
@@ -2270,7 +2474,7 @@
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" s="2">
         <v>2304</v>
@@ -2281,7 +2485,7 @@
       <c r="D18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="54">
         <v>256</v>
       </c>
       <c r="F18" s="27">
@@ -2291,19 +2495,23 @@
         <v>1620</v>
       </c>
       <c r="H18" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 36-42Mh/s</v>
       </c>
       <c r="I18">
         <v>39.799999999999997</v>
       </c>
-      <c r="M18" s="37"/>
+      <c r="J18" s="55">
+        <f t="shared" si="0"/>
+        <v>35.74934171587978</v>
+      </c>
+      <c r="M18" s="32"/>
       <c r="N18" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="31"/>
+      <c r="Q18" s="34"/>
       <c r="R18" s="17"/>
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
@@ -2311,7 +2519,7 @@
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19" s="2">
         <v>2560</v>
@@ -2332,34 +2540,35 @@
         <v>1770</v>
       </c>
       <c r="H19" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 36-42Mh/s</v>
       </c>
       <c r="I19">
         <v>46</v>
       </c>
-      <c r="J19" s="28">
-        <v>27</v>
-      </c>
-      <c r="M19" s="36" t="s">
+      <c r="J19" s="55">
+        <f t="shared" si="0"/>
+        <v>37.683114891284049</v>
+      </c>
+      <c r="M19" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="N19" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="N19" s="16" t="s">
-        <v>53</v>
-      </c>
       <c r="O19" s="16"/>
-      <c r="P19" s="30"/>
+      <c r="P19" s="33"/>
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
-      <c r="S19" s="30"/>
+      <c r="S19" s="33"/>
       <c r="T19" s="16"/>
       <c r="U19" s="10"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B20" s="2">
+        <v>111</v>
+      </c>
+      <c r="B20" s="51">
         <v>2944</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -2378,30 +2587,31 @@
         <v>1710</v>
       </c>
       <c r="H20" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36-44Mh/s</v>
       </c>
       <c r="I20">
         <v>47</v>
       </c>
-      <c r="J20" s="28">
-        <v>30.8</v>
-      </c>
-      <c r="M20" s="37"/>
+      <c r="J20" s="55">
+        <f t="shared" si="0"/>
+        <v>40.410638699433719</v>
+      </c>
+      <c r="M20" s="32"/>
       <c r="N20" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O20" s="17"/>
-      <c r="P20" s="31"/>
+      <c r="P20" s="34"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
-      <c r="S20" s="31"/>
+      <c r="S20" s="34"/>
       <c r="T20" s="17"/>
       <c r="U20" s="9"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2">
         <v>3072</v>
@@ -2422,18 +2632,22 @@
         <v>1815</v>
       </c>
       <c r="H21" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>36-44Mh/s</v>
+      </c>
+      <c r="J21" s="55">
         <f t="shared" si="0"/>
-        <v>36-44Mh/s</v>
-      </c>
-      <c r="M21" s="36" t="s">
+        <v>43.337714221176562</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="N21" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="O21" s="16"/>
       <c r="P21" s="16"/>
-      <c r="Q21" s="30"/>
+      <c r="Q21" s="33"/>
       <c r="R21" s="16"/>
       <c r="S21" s="16"/>
       <c r="T21" s="16"/>
@@ -2441,7 +2655,7 @@
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="2">
         <v>4352</v>
@@ -2462,16 +2676,20 @@
         <v>1545</v>
       </c>
       <c r="H22" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>50-57Mh/s</v>
+      </c>
+      <c r="J22" s="55">
         <f t="shared" si="0"/>
-        <v>50-57Mh/s</v>
-      </c>
-      <c r="M22" s="37"/>
+        <v>67.108932260131127</v>
+      </c>
+      <c r="M22" s="32"/>
       <c r="N22" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="31"/>
+      <c r="Q22" s="34"/>
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
       <c r="T22" s="17"/>
@@ -2499,19 +2717,22 @@
       <c r="G23" s="2">
         <v>1770</v>
       </c>
-      <c r="H23" s="29" t="e">
+      <c r="H23" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="J23" s="55">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M23" s="36" t="s">
+        <v>75.207991943115246</v>
+      </c>
+      <c r="M23" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="N23" s="16" t="s">
         <v>107</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>108</v>
       </c>
       <c r="O23" s="16"/>
       <c r="P23" s="16"/>
-      <c r="Q23" s="30"/>
+      <c r="Q23" s="33"/>
       <c r="R23" s="16"/>
       <c r="S23" s="16"/>
       <c r="T23" s="16"/>
@@ -2526,19 +2747,23 @@
       <c r="F24" s="27"/>
       <c r="G24" s="2"/>
       <c r="H24" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J24" s="55">
+        <f t="shared" ref="J24:J37" si="2">КОРЕНЬ(B24) * КОРЕНЬ(E24) * (КОРЕНЬ(F24) + 1) / 2000 * 4,2</f>
+        <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>238</v>
-      </c>
-      <c r="M24" s="37"/>
+        <v>234</v>
+      </c>
+      <c r="M24" s="32"/>
       <c r="N24" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="31"/>
+      <c r="Q24" s="34"/>
       <c r="R24" s="17"/>
       <c r="S24" s="17"/>
       <c r="T24" s="17"/>
@@ -2546,15 +2771,15 @@
     </row>
     <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2567,32 +2792,36 @@
         <v>11</v>
       </c>
       <c r="H25" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M25" s="36" t="s">
-        <v>109</v>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J25" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M25" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="N25" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O25" s="16"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
       <c r="R25" s="16"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="34"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="35"/>
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="24" t="s">
         <v>6</v>
       </c>
@@ -2603,19 +2832,23 @@
         <v>10</v>
       </c>
       <c r="H26" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M26" s="37"/>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J26" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M26" s="32"/>
       <c r="N26" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O26" s="17"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="31"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="34"/>
       <c r="R26" s="17"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="35"/>
+      <c r="S26" s="34"/>
+      <c r="T26" s="36"/>
       <c r="U26" s="9"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2623,8 +2856,8 @@
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="24" t="s">
         <v>7</v>
       </c>
@@ -2633,26 +2866,30 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M27" s="36" t="s">
-        <v>110</v>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J27" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M27" s="31" t="s">
+        <v>109</v>
       </c>
       <c r="N27" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O27" s="16"/>
       <c r="P27" s="16"/>
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
-      <c r="S27" s="30"/>
+      <c r="S27" s="33"/>
       <c r="T27" s="16"/>
       <c r="U27" s="10"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2">
         <v>896</v>
@@ -2673,24 +2910,28 @@
         <v>1665</v>
       </c>
       <c r="H28" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 14-16MH/s</v>
       </c>
-      <c r="M28" s="37"/>
+      <c r="J28" s="55">
+        <f t="shared" si="2"/>
+        <v>8.7572379969328473</v>
+      </c>
+      <c r="M28" s="32"/>
       <c r="N28" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
-      <c r="S28" s="31"/>
+      <c r="S28" s="34"/>
       <c r="T28" s="17"/>
       <c r="U28" s="9"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2">
         <v>1280</v>
@@ -2710,27 +2951,30 @@
       <c r="G29" s="2">
         <v>1725</v>
       </c>
-      <c r="H29" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M29" s="36" t="s">
-        <v>111</v>
+      <c r="H29" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="J29" s="55">
+        <f t="shared" si="2"/>
+        <v>12.628246111644353</v>
+      </c>
+      <c r="M29" s="31" t="s">
+        <v>110</v>
       </c>
       <c r="N29" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O29" s="16"/>
       <c r="P29" s="16"/>
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
-      <c r="S29" s="30"/>
+      <c r="S29" s="33"/>
       <c r="T29" s="16"/>
       <c r="U29" s="10"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2">
         <v>1408</v>
@@ -2744,31 +2988,35 @@
       <c r="E30" s="25">
         <v>192</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="50">
         <v>192</v>
       </c>
       <c r="G30" s="2">
         <v>1785</v>
       </c>
       <c r="H30" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 20-25Mh/s</v>
       </c>
-      <c r="M30" s="37"/>
+      <c r="J30" s="55">
+        <f t="shared" si="2"/>
+        <v>16.22127583646953</v>
+      </c>
+      <c r="M30" s="32"/>
       <c r="N30" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="17"/>
-      <c r="S30" s="31"/>
+      <c r="S30" s="34"/>
       <c r="T30" s="17"/>
       <c r="U30" s="9"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="2">
         <v>1408</v>
@@ -2782,33 +3030,37 @@
       <c r="E31" s="25">
         <v>192</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="50">
         <v>336</v>
       </c>
       <c r="G31" s="2">
         <v>1785</v>
       </c>
       <c r="H31" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25-31Mh/s</v>
       </c>
-      <c r="M31" s="36" t="s">
-        <v>112</v>
+      <c r="J31" s="55">
+        <f t="shared" si="2"/>
+        <v>21.106192417837129</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="N31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="34"/>
+        <v>60</v>
+      </c>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="33"/>
+      <c r="S31" s="33"/>
+      <c r="T31" s="35"/>
       <c r="U31" s="10"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="2">
         <v>1536</v>
@@ -2822,26 +3074,30 @@
       <c r="E32" s="25">
         <v>192</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="49">
         <v>288</v>
       </c>
       <c r="G32" s="2">
         <v>1770</v>
       </c>
       <c r="H32" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 24-31,5Mh/s</v>
       </c>
-      <c r="M32" s="37"/>
+      <c r="J32" s="55">
+        <f t="shared" si="2"/>
+        <v>20.494021816697664</v>
+      </c>
+      <c r="M32" s="32"/>
       <c r="N32" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="31"/>
-      <c r="S32" s="31"/>
-      <c r="T32" s="35"/>
+        <v>39</v>
+      </c>
+      <c r="O32" s="34"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="34"/>
+      <c r="R32" s="34"/>
+      <c r="S32" s="34"/>
+      <c r="T32" s="36"/>
       <c r="U32" s="9"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2853,34 +3109,38 @@
       <c r="F33" s="27"/>
       <c r="G33" s="2"/>
       <c r="H33" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M33" s="36" t="s">
-        <v>62</v>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J33" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="31" t="s">
+        <v>61</v>
       </c>
       <c r="N33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
+        <v>60</v>
+      </c>
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
       <c r="Q33" s="16"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
+      <c r="R33" s="33"/>
+      <c r="S33" s="33"/>
       <c r="T33" s="16"/>
       <c r="U33" s="10"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="44" t="s">
+      <c r="D34" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="24" t="s">
@@ -2893,30 +3153,34 @@
         <v>11</v>
       </c>
       <c r="H34" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M34" s="37"/>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J34" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M34" s="32"/>
       <c r="N34" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
+        <v>39</v>
+      </c>
+      <c r="O34" s="34"/>
+      <c r="P34" s="34"/>
       <c r="Q34" s="17"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="31"/>
+      <c r="R34" s="34"/>
+      <c r="S34" s="34"/>
       <c r="T34" s="17"/>
       <c r="U34" s="11"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="24" t="s">
         <v>6</v>
       </c>
@@ -2927,14 +3191,18 @@
         <v>10</v>
       </c>
       <c r="H35" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M35" s="36" t="s">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J35" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M35" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="N35" s="16" t="s">
         <v>113</v>
-      </c>
-      <c r="N35" s="16" t="s">
-        <v>114</v>
       </c>
       <c r="O35" s="16"/>
       <c r="P35" s="16"/>
@@ -2949,8 +3217,8 @@
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="24" t="s">
         <v>7</v>
       </c>
@@ -2959,12 +3227,16 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M36" s="37"/>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J36" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M36" s="32"/>
       <c r="N36" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O36" s="17"/>
       <c r="P36" s="17"/>
@@ -2976,7 +3248,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" s="2">
         <v>384</v>
@@ -2991,24 +3263,28 @@
         <v>64</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G37" s="2">
         <v>1468</v>
       </c>
       <c r="H37" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M37" s="36" t="s">
-        <v>66</v>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J37" s="55" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M37" s="31" t="s">
+        <v>65</v>
       </c>
       <c r="N37" s="16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O37" s="16"/>
       <c r="P37" s="16"/>
-      <c r="Q37" s="30"/>
+      <c r="Q37" s="33"/>
       <c r="R37" s="16"/>
       <c r="S37" s="16"/>
       <c r="T37" s="16"/>
@@ -3016,7 +3292,7 @@
     </row>
     <row r="38" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B38" s="2">
         <v>384</v>
@@ -3036,17 +3312,21 @@
       <c r="G38" s="2">
         <v>1468</v>
       </c>
-      <c r="H38" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M38" s="37"/>
+      <c r="H38" s="53"/>
+      <c r="I38">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J38" s="55">
+        <f>КОРЕНЬ(B38) * КОРЕНЬ(E38) * (КОРЕНЬ(F38) + 1) / 2000 * 4,2</f>
+        <v>2.6100550548253865</v>
+      </c>
+      <c r="M38" s="32"/>
       <c r="N38" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O38" s="17"/>
       <c r="P38" s="17"/>
-      <c r="Q38" s="31"/>
+      <c r="Q38" s="34"/>
       <c r="R38" s="17"/>
       <c r="S38" s="17"/>
       <c r="T38" s="17"/>
@@ -3054,7 +3334,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B39" s="2">
         <v>640</v>
@@ -3075,26 +3355,30 @@
         <v>1455</v>
       </c>
       <c r="H39" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M39" s="36" t="s">
-        <v>67</v>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J39" s="55">
+        <f t="shared" ref="J39:J47" si="3">КОРЕНЬ(B39) * КОРЕНЬ(E39) * (КОРЕНЬ(F39) + 1) / 2000 * 4,2</f>
+        <v>6.9620240551406516</v>
+      </c>
+      <c r="M39" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
-      <c r="S39" s="30"/>
-      <c r="T39" s="34"/>
+        <v>205</v>
+      </c>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="33"/>
+      <c r="S39" s="33"/>
+      <c r="T39" s="35"/>
       <c r="U39" s="9"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B40" s="2">
         <v>768</v>
@@ -3115,24 +3399,28 @@
         <v>1518</v>
       </c>
       <c r="H40" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M40" s="37"/>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J40" s="55">
+        <f t="shared" si="3"/>
+        <v>5.79628020754493</v>
+      </c>
+      <c r="M40" s="32"/>
       <c r="N40" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-      <c r="Q40" s="31"/>
-      <c r="R40" s="31"/>
-      <c r="S40" s="31"/>
-      <c r="T40" s="35"/>
+        <v>35</v>
+      </c>
+      <c r="O40" s="34"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="34"/>
+      <c r="T40" s="36"/>
       <c r="U40" s="10"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B41" s="2">
         <v>768</v>
@@ -3153,26 +3441,30 @@
         <v>1392</v>
       </c>
       <c r="H41" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15Mh/s</v>
       </c>
-      <c r="M41" s="36" t="s">
+      <c r="J41" s="55">
+        <f t="shared" si="3"/>
+        <v>7.6265152417882511</v>
+      </c>
+      <c r="M41" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="N41" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="N41" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="O41" s="30"/>
+      <c r="O41" s="33"/>
       <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
       <c r="S41" s="16"/>
-      <c r="T41" s="34"/>
+      <c r="T41" s="35"/>
       <c r="U41" s="9"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B42" s="2">
         <v>1152</v>
@@ -3193,24 +3485,28 @@
         <v>1708</v>
       </c>
       <c r="H42" s="29" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M42" s="37"/>
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J42" s="55">
+        <f t="shared" si="3"/>
+        <v>14.672696064662142</v>
+      </c>
+      <c r="M42" s="32"/>
       <c r="N42" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="O42" s="31"/>
+        <v>35</v>
+      </c>
+      <c r="O42" s="34"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="17"/>
       <c r="R42" s="17"/>
       <c r="S42" s="17"/>
-      <c r="T42" s="35"/>
+      <c r="T42" s="36"/>
       <c r="U42" s="10"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B43" s="2">
         <v>1280</v>
@@ -3231,28 +3527,32 @@
         <v>1708</v>
       </c>
       <c r="H43" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17-23Mh/s</v>
       </c>
-      <c r="M43" s="36" t="s">
-        <v>70</v>
+      <c r="J43" s="55">
+        <f t="shared" si="3"/>
+        <v>15.466379659907197</v>
+      </c>
+      <c r="M43" s="31" t="s">
+        <v>69</v>
       </c>
       <c r="N43" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="O43" s="30"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="30"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="34"/>
+        <v>114</v>
+      </c>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="33"/>
+      <c r="S43" s="33"/>
+      <c r="T43" s="35"/>
       <c r="U43" s="9"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="2">
+        <v>101</v>
+      </c>
+      <c r="B44" s="52">
         <v>1920</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -3271,26 +3571,30 @@
         <v>1683</v>
       </c>
       <c r="H44" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 24-28Mh/s120W</v>
       </c>
-      <c r="M44" s="37"/>
+      <c r="J44" s="55">
+        <f t="shared" si="3"/>
+        <v>25.028729987756073</v>
+      </c>
+      <c r="M44" s="32"/>
       <c r="N44" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="O44" s="31"/>
-      <c r="P44" s="31"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="31"/>
-      <c r="S44" s="31"/>
-      <c r="T44" s="35"/>
+        <v>35</v>
+      </c>
+      <c r="O44" s="34"/>
+      <c r="P44" s="34"/>
+      <c r="Q44" s="34"/>
+      <c r="R44" s="34"/>
+      <c r="S44" s="34"/>
+      <c r="T44" s="36"/>
       <c r="U44" s="10"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="2">
+        <v>36</v>
+      </c>
+      <c r="B45" s="52">
         <v>2432</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -3302,33 +3606,37 @@
       <c r="E45" s="25">
         <v>256</v>
       </c>
-      <c r="F45" s="27">
+      <c r="F45" s="49">
         <v>256</v>
       </c>
       <c r="G45" s="2">
         <v>1683</v>
       </c>
       <c r="H45" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 25-29Mh/s</v>
       </c>
-      <c r="M45" s="36" t="s">
+      <c r="J45" s="55">
+        <f t="shared" si="3"/>
+        <v>28.168906227967039</v>
+      </c>
+      <c r="M45" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="N45" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="N45" s="16" t="s">
-        <v>72</v>
       </c>
       <c r="O45" s="16"/>
       <c r="P45" s="16"/>
       <c r="Q45" s="16"/>
       <c r="R45" s="16"/>
-      <c r="S45" s="30"/>
+      <c r="S45" s="33"/>
       <c r="T45" s="16"/>
       <c r="U45" s="9"/>
     </row>
     <row r="46" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" s="2">
         <v>2560</v>
@@ -3342,31 +3650,35 @@
       <c r="E46" s="25">
         <v>256</v>
       </c>
-      <c r="F46" s="27">
+      <c r="F46" s="49">
         <v>320</v>
       </c>
       <c r="G46" s="2">
         <v>1733</v>
       </c>
       <c r="H46" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30-37Mh/s</v>
       </c>
-      <c r="M46" s="37"/>
+      <c r="J46" s="55">
+        <f t="shared" si="3"/>
+        <v>32.111288915377564</v>
+      </c>
+      <c r="M46" s="32"/>
       <c r="N46" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O46" s="17"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="17"/>
       <c r="R46" s="17"/>
-      <c r="S46" s="31"/>
+      <c r="S46" s="34"/>
       <c r="T46" s="17"/>
       <c r="U46" s="10"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B47" s="2">
         <v>3584</v>
@@ -3387,26 +3699,30 @@
         <v>1582</v>
       </c>
       <c r="H47" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v> 40-50Mh/s</v>
       </c>
-      <c r="M47" s="36" t="s">
-        <v>74</v>
+      <c r="J47" s="55">
+        <f t="shared" si="3"/>
+        <v>54.250339828613058</v>
+      </c>
+      <c r="M47" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="N47" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="O47" s="30"/>
-      <c r="P47" s="30"/>
-      <c r="Q47" s="30"/>
-      <c r="R47" s="30"/>
-      <c r="S47" s="30"/>
-      <c r="T47" s="34"/>
+        <v>114</v>
+      </c>
+      <c r="O47" s="33"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="33"/>
+      <c r="S47" s="33"/>
+      <c r="T47" s="35"/>
       <c r="U47" s="9"/>
     </row>
     <row r="48" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>1</v>
@@ -3427,24 +3743,24 @@
         <v>11</v>
       </c>
       <c r="H48" s="29" t="e">
-        <f>VLOOKUP(A48,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M48" s="37"/>
+        <f t="shared" ref="H48:H79" si="4">ВПР(A48;M:N;2;0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M48" s="32"/>
       <c r="N48" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O48" s="31"/>
-      <c r="P48" s="31"/>
-      <c r="Q48" s="31"/>
-      <c r="R48" s="31"/>
-      <c r="S48" s="31"/>
-      <c r="T48" s="35"/>
+        <v>72</v>
+      </c>
+      <c r="O48" s="34"/>
+      <c r="P48" s="34"/>
+      <c r="Q48" s="34"/>
+      <c r="R48" s="34"/>
+      <c r="S48" s="34"/>
+      <c r="T48" s="36"/>
       <c r="U48" s="10"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>2</v>
@@ -3461,20 +3777,20 @@
         <v>10</v>
       </c>
       <c r="H49" s="29" t="e">
-        <f>VLOOKUP(A49,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M49" s="36" t="s">
-        <v>75</v>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M49" s="31" t="s">
+        <v>74</v>
       </c>
       <c r="N49" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="O49" s="30"/>
-      <c r="P49" s="30"/>
-      <c r="Q49" s="30"/>
+        <v>115</v>
+      </c>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
       <c r="R49" s="16"/>
-      <c r="S49" s="30"/>
+      <c r="S49" s="33"/>
       <c r="T49" s="16"/>
       <c r="U49" s="9"/>
     </row>
@@ -3493,24 +3809,24 @@
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="29" t="e">
-        <f>VLOOKUP(A50,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M50" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M50" s="32"/>
       <c r="N50" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="O50" s="31"/>
-      <c r="P50" s="31"/>
-      <c r="Q50" s="31"/>
+        <v>116</v>
+      </c>
+      <c r="O50" s="34"/>
+      <c r="P50" s="34"/>
+      <c r="Q50" s="34"/>
       <c r="R50" s="17"/>
-      <c r="S50" s="31"/>
+      <c r="S50" s="34"/>
       <c r="T50" s="17"/>
       <c r="U50" s="10"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B51" s="5">
         <v>768</v>
@@ -3525,32 +3841,32 @@
         <v>128</v>
       </c>
       <c r="F51" s="27" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G51" s="5">
         <v>1188</v>
       </c>
       <c r="H51" s="29" t="e">
-        <f>VLOOKUP(A51,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M51" s="36" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M51" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="N51" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="N51" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="O51" s="30"/>
-      <c r="P51" s="30"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="33"/>
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
-      <c r="S51" s="30"/>
+      <c r="S51" s="33"/>
       <c r="T51" s="16"/>
       <c r="U51" s="9"/>
     </row>
     <row r="52" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B52" s="5">
         <v>1024</v>
@@ -3571,24 +3887,24 @@
         <v>1178</v>
       </c>
       <c r="H52" s="29" t="e">
-        <f>VLOOKUP(A52,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M52" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M52" s="32"/>
       <c r="N52" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="O52" s="31"/>
-      <c r="P52" s="31"/>
+        <v>77</v>
+      </c>
+      <c r="O52" s="34"/>
+      <c r="P52" s="34"/>
       <c r="Q52" s="17"/>
       <c r="R52" s="17"/>
-      <c r="S52" s="31"/>
+      <c r="S52" s="34"/>
       <c r="T52" s="17"/>
       <c r="U52" s="10"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B53" s="5">
         <v>1644</v>
@@ -3609,26 +3925,26 @@
         <v>1178</v>
       </c>
       <c r="H53" s="29" t="e">
-        <f>VLOOKUP(A53,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M53" s="36" t="s">
-        <v>79</v>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M53" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="N53" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="O53" s="30"/>
-      <c r="P53" s="30"/>
-      <c r="Q53" s="30"/>
-      <c r="R53" s="30"/>
-      <c r="S53" s="30"/>
-      <c r="T53" s="34"/>
+        <v>117</v>
+      </c>
+      <c r="O53" s="33"/>
+      <c r="P53" s="33"/>
+      <c r="Q53" s="33"/>
+      <c r="R53" s="33"/>
+      <c r="S53" s="33"/>
+      <c r="T53" s="35"/>
       <c r="U53" s="9"/>
     </row>
     <row r="54" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B54" s="5">
         <v>2048</v>
@@ -3649,24 +3965,24 @@
         <v>1216</v>
       </c>
       <c r="H54" s="29" t="e">
-        <f>VLOOKUP(A54,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M54" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M54" s="32"/>
       <c r="N54" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="O54" s="31"/>
-      <c r="P54" s="31"/>
-      <c r="Q54" s="31"/>
-      <c r="R54" s="31"/>
-      <c r="S54" s="31"/>
-      <c r="T54" s="35"/>
+        <v>77</v>
+      </c>
+      <c r="O54" s="34"/>
+      <c r="P54" s="34"/>
+      <c r="Q54" s="34"/>
+      <c r="R54" s="34"/>
+      <c r="S54" s="34"/>
+      <c r="T54" s="36"/>
       <c r="U54" s="10"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B55" s="5">
         <v>2816</v>
@@ -3681,26 +3997,26 @@
         <v>384</v>
       </c>
       <c r="F55" s="27" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G55" s="5">
         <v>1075</v>
       </c>
       <c r="H55" s="29" t="e">
-        <f>VLOOKUP(A55,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M55" s="36" t="s">
-        <v>80</v>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M55" s="31" t="s">
+        <v>79</v>
       </c>
       <c r="N55" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="O55" s="16"/>
-      <c r="P55" s="30"/>
+      <c r="P55" s="33"/>
       <c r="Q55" s="16"/>
       <c r="R55" s="16"/>
-      <c r="S55" s="30"/>
+      <c r="S55" s="33"/>
       <c r="T55" s="16"/>
       <c r="U55" s="9"/>
     </row>
@@ -3713,24 +4029,24 @@
       <c r="F56" s="27"/>
       <c r="G56" s="5"/>
       <c r="H56" s="29" t="e">
-        <f>VLOOKUP(A56,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M56" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M56" s="32"/>
       <c r="N56" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O56" s="17"/>
-      <c r="P56" s="31"/>
+      <c r="P56" s="34"/>
       <c r="Q56" s="17"/>
       <c r="R56" s="17"/>
-      <c r="S56" s="31"/>
+      <c r="S56" s="34"/>
       <c r="T56" s="17"/>
       <c r="U56" s="10"/>
     </row>
     <row r="57" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>1</v>
@@ -3751,16 +4067,16 @@
         <v>11</v>
       </c>
       <c r="H57" s="29" t="e">
-        <f>VLOOKUP(A57,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M57" s="36" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M57" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="N57" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="N57" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="O57" s="30"/>
+      <c r="O57" s="33"/>
       <c r="P57" s="16"/>
       <c r="Q57" s="16"/>
       <c r="R57" s="16"/>
@@ -3770,7 +4086,7 @@
     </row>
     <row r="58" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>2</v>
@@ -3787,14 +4103,14 @@
         <v>10</v>
       </c>
       <c r="H58" s="29" t="e">
-        <f>VLOOKUP(A58,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M58" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M58" s="32"/>
       <c r="N58" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="O58" s="31"/>
+        <v>80</v>
+      </c>
+      <c r="O58" s="34"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="17"/>
       <c r="R58" s="17"/>
@@ -3817,26 +4133,26 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="29" t="e">
-        <f>VLOOKUP(A59,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M59" s="36" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M59" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="N59" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="N59" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="O59" s="30"/>
-      <c r="P59" s="30"/>
-      <c r="Q59" s="30"/>
-      <c r="R59" s="30"/>
-      <c r="S59" s="30"/>
+      <c r="O59" s="33"/>
+      <c r="P59" s="33"/>
+      <c r="Q59" s="33"/>
+      <c r="R59" s="33"/>
+      <c r="S59" s="33"/>
       <c r="T59" s="16"/>
-      <c r="U59" s="40"/>
+      <c r="U59" s="37"/>
     </row>
     <row r="60" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B60" s="5">
         <v>192</v>
@@ -3855,24 +4171,24 @@
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="29" t="e">
-        <f>VLOOKUP(A60,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M60" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M60" s="32"/>
       <c r="N60" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="O60" s="31"/>
-      <c r="P60" s="31"/>
-      <c r="Q60" s="31"/>
-      <c r="R60" s="31"/>
-      <c r="S60" s="31"/>
+        <v>32</v>
+      </c>
+      <c r="O60" s="34"/>
+      <c r="P60" s="34"/>
+      <c r="Q60" s="34"/>
+      <c r="R60" s="34"/>
+      <c r="S60" s="34"/>
       <c r="T60" s="17"/>
-      <c r="U60" s="41"/>
+      <c r="U60" s="38"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B61" s="5">
         <v>192</v>
@@ -3891,26 +4207,26 @@
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="29" t="e">
-        <f>VLOOKUP(A61,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M61" s="36" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M61" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="N61" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="N61" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="O61" s="30"/>
-      <c r="P61" s="30"/>
-      <c r="Q61" s="30"/>
+      <c r="O61" s="33"/>
+      <c r="P61" s="33"/>
+      <c r="Q61" s="33"/>
       <c r="R61" s="16"/>
-      <c r="S61" s="30"/>
+      <c r="S61" s="33"/>
       <c r="T61" s="16"/>
       <c r="U61" s="9"/>
     </row>
     <row r="62" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B62" s="5">
         <v>96</v>
@@ -3929,24 +4245,24 @@
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="29" t="e">
-        <f>VLOOKUP(A62,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M62" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M62" s="32"/>
       <c r="N62" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="O62" s="31"/>
-      <c r="P62" s="31"/>
-      <c r="Q62" s="31"/>
+        <v>57</v>
+      </c>
+      <c r="O62" s="34"/>
+      <c r="P62" s="34"/>
+      <c r="Q62" s="34"/>
       <c r="R62" s="17"/>
-      <c r="S62" s="31"/>
+      <c r="S62" s="34"/>
       <c r="T62" s="17"/>
       <c r="U62" s="10"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B63" s="5">
         <v>384</v>
@@ -3965,26 +4281,26 @@
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="29" t="e">
-        <f>VLOOKUP(A63,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M63" s="36" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M63" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="N63" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="N63" s="16" t="s">
-        <v>89</v>
       </c>
       <c r="O63" s="16"/>
       <c r="P63" s="16"/>
-      <c r="Q63" s="30"/>
+      <c r="Q63" s="33"/>
       <c r="R63" s="16"/>
-      <c r="S63" s="30"/>
+      <c r="S63" s="33"/>
       <c r="T63" s="16"/>
       <c r="U63" s="9"/>
     </row>
     <row r="64" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B64" s="5">
         <v>384</v>
@@ -4003,24 +4319,24 @@
       </c>
       <c r="G64" s="5"/>
       <c r="H64" s="29" t="e">
-        <f>VLOOKUP(A64,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M64" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M64" s="32"/>
       <c r="N64" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O64" s="17"/>
       <c r="P64" s="17"/>
-      <c r="Q64" s="31"/>
+      <c r="Q64" s="34"/>
       <c r="R64" s="17"/>
-      <c r="S64" s="31"/>
+      <c r="S64" s="34"/>
       <c r="T64" s="17"/>
       <c r="U64" s="10"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B65" s="5">
         <v>384</v>
@@ -4039,26 +4355,26 @@
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="29" t="e">
-        <f>VLOOKUP(A65,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M65" s="36" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M65" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="N65" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="N65" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="O65" s="30"/>
-      <c r="P65" s="30"/>
-      <c r="Q65" s="30"/>
-      <c r="R65" s="30"/>
-      <c r="S65" s="30"/>
-      <c r="T65" s="34"/>
+      <c r="O65" s="33"/>
+      <c r="P65" s="33"/>
+      <c r="Q65" s="33"/>
+      <c r="R65" s="33"/>
+      <c r="S65" s="33"/>
+      <c r="T65" s="35"/>
       <c r="U65" s="9"/>
     </row>
     <row r="66" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B66" s="5">
         <v>384</v>
@@ -4077,24 +4393,24 @@
       </c>
       <c r="G66" s="5"/>
       <c r="H66" s="29" t="e">
-        <f>VLOOKUP(A66,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M66" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M66" s="32"/>
       <c r="N66" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="O66" s="31"/>
-      <c r="P66" s="31"/>
-      <c r="Q66" s="31"/>
-      <c r="R66" s="31"/>
-      <c r="S66" s="31"/>
-      <c r="T66" s="35"/>
+        <v>91</v>
+      </c>
+      <c r="O66" s="34"/>
+      <c r="P66" s="34"/>
+      <c r="Q66" s="34"/>
+      <c r="R66" s="34"/>
+      <c r="S66" s="34"/>
+      <c r="T66" s="36"/>
       <c r="U66" s="10"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B67" s="5">
         <v>384</v>
@@ -4113,18 +4429,18 @@
       </c>
       <c r="G67" s="5"/>
       <c r="H67" s="29" t="e">
-        <f>VLOOKUP(A67,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M67" s="36" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M67" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="N67" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="N67" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="O67" s="30"/>
-      <c r="P67" s="30"/>
-      <c r="Q67" s="30"/>
+      <c r="O67" s="33"/>
+      <c r="P67" s="33"/>
+      <c r="Q67" s="33"/>
       <c r="R67" s="16"/>
       <c r="S67" s="16"/>
       <c r="T67" s="16"/>
@@ -4132,7 +4448,7 @@
     </row>
     <row r="68" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B68" s="5">
         <v>512</v>
@@ -4153,16 +4469,16 @@
         <v>1085</v>
       </c>
       <c r="H68" s="29" t="e">
-        <f>VLOOKUP(A68,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M68" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M68" s="32"/>
       <c r="N68" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="O68" s="31"/>
-      <c r="P68" s="31"/>
-      <c r="Q68" s="31"/>
+        <v>42</v>
+      </c>
+      <c r="O68" s="34"/>
+      <c r="P68" s="34"/>
+      <c r="Q68" s="34"/>
       <c r="R68" s="17"/>
       <c r="S68" s="17"/>
       <c r="T68" s="17"/>
@@ -4170,7 +4486,7 @@
     </row>
     <row r="69" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B69" s="5">
         <v>640</v>
@@ -4185,32 +4501,32 @@
         <v>128</v>
       </c>
       <c r="F69" s="27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G69" s="5">
         <v>1085</v>
       </c>
       <c r="H69" s="29" t="e">
-        <f>VLOOKUP(A69,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M69" s="36" t="s">
-        <v>95</v>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M69" s="31" t="s">
+        <v>94</v>
       </c>
       <c r="N69" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="O69" s="30"/>
-      <c r="P69" s="30"/>
-      <c r="Q69" s="30"/>
-      <c r="R69" s="30"/>
-      <c r="S69" s="30"/>
+        <v>59</v>
+      </c>
+      <c r="O69" s="33"/>
+      <c r="P69" s="33"/>
+      <c r="Q69" s="33"/>
+      <c r="R69" s="33"/>
+      <c r="S69" s="33"/>
       <c r="T69" s="16"/>
       <c r="U69" s="9"/>
     </row>
     <row r="70" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B70" s="5">
         <v>1152</v>
@@ -4225,30 +4541,30 @@
         <v>256</v>
       </c>
       <c r="F70" s="27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G70" s="5">
         <v>1033</v>
       </c>
       <c r="H70" s="29" t="e">
-        <f>VLOOKUP(A70,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M70" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M70" s="32"/>
       <c r="N70" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="O70" s="31"/>
-      <c r="P70" s="31"/>
-      <c r="Q70" s="31"/>
-      <c r="R70" s="31"/>
-      <c r="S70" s="31"/>
+        <v>46</v>
+      </c>
+      <c r="O70" s="34"/>
+      <c r="P70" s="34"/>
+      <c r="Q70" s="34"/>
+      <c r="R70" s="34"/>
+      <c r="S70" s="34"/>
       <c r="T70" s="17"/>
       <c r="U70" s="10"/>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B71" s="3">
         <v>1152</v>
@@ -4269,26 +4585,26 @@
         <v>888</v>
       </c>
       <c r="H71" s="29" t="e">
-        <f>VLOOKUP(A71,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M71" s="36" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M71" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="N71" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="N71" s="16" t="s">
-        <v>98</v>
       </c>
       <c r="O71" s="16"/>
       <c r="P71" s="16"/>
-      <c r="Q71" s="30"/>
-      <c r="R71" s="30"/>
-      <c r="S71" s="30"/>
+      <c r="Q71" s="33"/>
+      <c r="R71" s="33"/>
+      <c r="S71" s="33"/>
       <c r="T71" s="16"/>
       <c r="U71" s="9"/>
     </row>
     <row r="72" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B72" s="3">
         <v>1344</v>
@@ -4303,30 +4619,30 @@
         <v>256</v>
       </c>
       <c r="F72" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G72" s="3">
         <v>1033</v>
       </c>
       <c r="H72" s="29" t="e">
-        <f>VLOOKUP(A72,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M72" s="37"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M72" s="32"/>
       <c r="N72" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O72" s="17"/>
       <c r="P72" s="17"/>
-      <c r="Q72" s="31"/>
-      <c r="R72" s="31"/>
-      <c r="S72" s="31"/>
+      <c r="Q72" s="34"/>
+      <c r="R72" s="34"/>
+      <c r="S72" s="34"/>
       <c r="T72" s="17"/>
       <c r="U72" s="10"/>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B73" s="5">
         <v>1536</v>
@@ -4341,31 +4657,31 @@
         <v>256</v>
       </c>
       <c r="F73" s="27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G73" s="5">
         <v>1085</v>
       </c>
       <c r="H73" s="29" t="e">
-        <f>VLOOKUP(A73,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M73" s="42" t="s">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M73" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="N73" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="N73" s="18" t="s">
-        <v>100</v>
       </c>
       <c r="O73" s="18"/>
       <c r="P73" s="18"/>
-      <c r="Q73" s="32"/>
-      <c r="R73" s="32"/>
+      <c r="Q73" s="41"/>
+      <c r="R73" s="41"/>
       <c r="T73" s="20"/>
       <c r="U73" s="9"/>
     </row>
     <row r="74" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B74" s="5">
         <v>2304</v>
@@ -4380,30 +4696,30 @@
         <v>384</v>
       </c>
       <c r="F74" s="27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G74" s="5">
         <v>900</v>
       </c>
       <c r="H74" s="29" t="e">
-        <f>VLOOKUP(A74,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M74" s="43"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M74" s="40"/>
       <c r="N74" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O74" s="19"/>
       <c r="P74" s="19"/>
-      <c r="Q74" s="33"/>
-      <c r="R74" s="33"/>
+      <c r="Q74" s="42"/>
+      <c r="R74" s="42"/>
       <c r="S74" s="21"/>
       <c r="T74" s="22"/>
       <c r="U74" s="10"/>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B75" s="5">
         <v>2880</v>
@@ -4424,16 +4740,16 @@
         <v>928</v>
       </c>
       <c r="H75" s="29" t="e">
-        <f>VLOOKUP(A75,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M75" s="40"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M75" s="37"/>
       <c r="N75" s="6"/>
-      <c r="O75" s="40"/>
-      <c r="P75" s="40"/>
-      <c r="Q75" s="40"/>
+      <c r="O75" s="37"/>
+      <c r="P75" s="37"/>
+      <c r="Q75" s="37"/>
       <c r="R75" s="6"/>
-      <c r="S75" s="40"/>
+      <c r="S75" s="37"/>
       <c r="T75" s="6"/>
       <c r="U75" s="9"/>
     </row>
@@ -4446,22 +4762,22 @@
       <c r="F76" s="27"/>
       <c r="G76" s="5"/>
       <c r="H76" s="29" t="e">
-        <f>VLOOKUP(A76,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M76" s="41"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M76" s="38"/>
       <c r="N76" s="7"/>
-      <c r="O76" s="41"/>
-      <c r="P76" s="41"/>
-      <c r="Q76" s="41"/>
+      <c r="O76" s="38"/>
+      <c r="P76" s="38"/>
+      <c r="Q76" s="38"/>
       <c r="R76" s="7"/>
-      <c r="S76" s="41"/>
+      <c r="S76" s="38"/>
       <c r="T76" s="7"/>
       <c r="U76" s="10"/>
     </row>
     <row r="77" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>1</v>
@@ -4482,22 +4798,22 @@
         <v>11</v>
       </c>
       <c r="H77" s="29" t="e">
-        <f>VLOOKUP(A77,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M77" s="40"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M77" s="37"/>
       <c r="N77" s="6"/>
-      <c r="O77" s="40"/>
-      <c r="P77" s="40"/>
-      <c r="Q77" s="40"/>
-      <c r="R77" s="40"/>
-      <c r="S77" s="40"/>
-      <c r="T77" s="40"/>
+      <c r="O77" s="37"/>
+      <c r="P77" s="37"/>
+      <c r="Q77" s="37"/>
+      <c r="R77" s="37"/>
+      <c r="S77" s="37"/>
+      <c r="T77" s="37"/>
       <c r="U77" s="9"/>
     </row>
     <row r="78" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>2</v>
@@ -4514,17 +4830,17 @@
         <v>10</v>
       </c>
       <c r="H78" s="29" t="e">
-        <f>VLOOKUP(A78,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M78" s="41"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M78" s="38"/>
       <c r="N78" s="7"/>
-      <c r="O78" s="41"/>
-      <c r="P78" s="41"/>
-      <c r="Q78" s="41"/>
-      <c r="R78" s="41"/>
-      <c r="S78" s="41"/>
-      <c r="T78" s="41"/>
+      <c r="O78" s="38"/>
+      <c r="P78" s="38"/>
+      <c r="Q78" s="38"/>
+      <c r="R78" s="38"/>
+      <c r="S78" s="38"/>
+      <c r="T78" s="38"/>
       <c r="U78" s="10"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
@@ -4542,22 +4858,22 @@
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="29" t="e">
-        <f>VLOOKUP(A79,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M79" s="40"/>
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M79" s="37"/>
       <c r="N79" s="6"/>
       <c r="O79" s="6"/>
       <c r="P79" s="6"/>
-      <c r="Q79" s="40"/>
-      <c r="R79" s="40"/>
-      <c r="S79" s="40"/>
-      <c r="T79" s="40"/>
+      <c r="Q79" s="37"/>
+      <c r="R79" s="37"/>
+      <c r="S79" s="37"/>
+      <c r="T79" s="37"/>
       <c r="U79" s="9"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B80" s="3">
         <v>48</v>
@@ -4578,22 +4894,22 @@
         <v>1046</v>
       </c>
       <c r="H80" s="29" t="e">
-        <f>VLOOKUP(A80,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M80" s="41"/>
+        <f t="shared" ref="H80:H111" si="5">ВПР(A80;M:N;2;0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M80" s="38"/>
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
       <c r="P80" s="7"/>
-      <c r="Q80" s="41"/>
-      <c r="R80" s="41"/>
-      <c r="S80" s="41"/>
-      <c r="T80" s="41"/>
+      <c r="Q80" s="38"/>
+      <c r="R80" s="38"/>
+      <c r="S80" s="38"/>
+      <c r="T80" s="38"/>
       <c r="U80" s="10"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B81" s="5">
         <v>48</v>
@@ -4614,22 +4930,22 @@
         <v>900</v>
       </c>
       <c r="H81" s="29" t="e">
-        <f>VLOOKUP(A81,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M81" s="38"/>
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M81" s="43"/>
       <c r="N81" s="8"/>
       <c r="O81" s="8"/>
       <c r="P81" s="8"/>
-      <c r="Q81" s="38"/>
-      <c r="R81" s="38"/>
-      <c r="S81" s="38"/>
-      <c r="T81" s="38"/>
+      <c r="Q81" s="43"/>
+      <c r="R81" s="43"/>
+      <c r="S81" s="43"/>
+      <c r="T81" s="43"/>
       <c r="U81" s="12"/>
     </row>
     <row r="82" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B82" s="3">
         <v>48</v>
@@ -4650,22 +4966,22 @@
         <v>1620</v>
       </c>
       <c r="H82" s="29" t="e">
-        <f>VLOOKUP(A82,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M82" s="39"/>
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M82" s="44"/>
       <c r="N82" s="13"/>
       <c r="O82" s="13"/>
       <c r="P82" s="13"/>
-      <c r="Q82" s="39"/>
-      <c r="R82" s="39"/>
-      <c r="S82" s="39"/>
-      <c r="T82" s="39"/>
+      <c r="Q82" s="44"/>
+      <c r="R82" s="44"/>
+      <c r="S82" s="44"/>
+      <c r="T82" s="44"/>
       <c r="U82" s="14"/>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B83" s="5">
         <v>96</v>
@@ -4686,13 +5002,13 @@
         <v>1400</v>
       </c>
       <c r="H83" s="29" t="e">
-        <f>VLOOKUP(A83,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B84" s="3">
         <v>192</v>
@@ -4713,13 +5029,13 @@
         <v>875</v>
       </c>
       <c r="H84" s="29" t="e">
-        <f>VLOOKUP(A84,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B85" s="5">
         <v>96</v>
@@ -4740,13 +5056,13 @@
         <v>1620</v>
       </c>
       <c r="H85" s="29" t="e">
-        <f>VLOOKUP(A85,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B86" s="5">
         <v>96</v>
@@ -4761,19 +5077,19 @@
         <v>128</v>
       </c>
       <c r="F86" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G86" s="5">
         <v>1620</v>
       </c>
       <c r="H86" s="29" t="e">
-        <f>VLOOKUP(A86,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B87" s="5">
         <v>384</v>
@@ -4794,13 +5110,13 @@
         <v>900</v>
       </c>
       <c r="H87" s="29" t="e">
-        <f>VLOOKUP(A87,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B88" s="3">
         <v>384</v>
@@ -4821,13 +5137,13 @@
         <v>797</v>
       </c>
       <c r="H88" s="29" t="e">
-        <f>VLOOKUP(A88,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="89" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B89" s="3">
         <v>144</v>
@@ -4848,13 +5164,13 @@
         <v>1440</v>
       </c>
       <c r="H89" s="29" t="e">
-        <f>VLOOKUP(A89,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B90" s="3">
         <v>384</v>
@@ -4875,13 +5191,13 @@
         <v>950</v>
       </c>
       <c r="H90" s="29" t="e">
-        <f>VLOOKUP(A90,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B91" s="3">
         <v>288</v>
@@ -4896,19 +5212,19 @@
         <v>192</v>
       </c>
       <c r="F91" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G91" s="3">
         <v>1552</v>
       </c>
       <c r="H91" s="29" t="e">
-        <f>VLOOKUP(A91,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B92" s="5">
         <v>384</v>
@@ -4929,13 +5245,13 @@
         <v>1058</v>
       </c>
       <c r="H92" s="29" t="e">
-        <f>VLOOKUP(A92,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B93" s="5">
         <v>768</v>
@@ -4950,19 +5266,19 @@
         <v>128</v>
       </c>
       <c r="F93" s="27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G93" s="5">
         <v>928</v>
       </c>
       <c r="H93" s="29" t="e">
-        <f>VLOOKUP(A93,M:N,2,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="94" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B94" s="5">
         <v>768</v>
@@ -4977,13 +5293,13 @@
         <v>192</v>
       </c>
       <c r="F94" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H94" s="29" t="e">
-        <f>VLOOKUP(A94,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -4996,13 +5312,13 @@
       <c r="F95" s="27"/>
       <c r="G95" s="5"/>
       <c r="H95" s="29" t="e">
-        <f>VLOOKUP(A95,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B96" s="5">
         <v>960</v>
@@ -5017,19 +5333,19 @@
         <v>192</v>
       </c>
       <c r="F96" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G96" s="5">
         <v>980</v>
       </c>
       <c r="H96" s="29" t="e">
-        <f>VLOOKUP(A96,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B97" s="3">
         <v>1152</v>
@@ -5050,13 +5366,13 @@
         <v>823</v>
       </c>
       <c r="H97" s="29" t="e">
-        <f>VLOOKUP(A97,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B98" s="5">
         <v>1344</v>
@@ -5071,19 +5387,19 @@
         <v>192</v>
       </c>
       <c r="F98" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G98" s="5">
         <v>980</v>
       </c>
       <c r="H98" s="29" t="e">
-        <f>VLOOKUP(A98,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B99" s="5">
         <v>1344</v>
@@ -5098,19 +5414,19 @@
         <v>256</v>
       </c>
       <c r="F99" s="27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G99" s="5">
         <v>980</v>
       </c>
       <c r="H99" s="29" t="e">
-        <f>VLOOKUP(A99,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B100" s="5">
         <v>1536</v>
@@ -5125,19 +5441,19 @@
         <v>256</v>
       </c>
       <c r="F100" s="27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G100" s="5">
         <v>1006</v>
       </c>
       <c r="H100" s="29" t="e">
-        <f>VLOOKUP(A100,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B101" s="5">
         <v>3072</v>
@@ -5149,7 +5465,7 @@
         <v>27</v>
       </c>
       <c r="E101" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F101" s="27">
         <v>384</v>
@@ -5158,13 +5474,13 @@
         <v>915</v>
       </c>
       <c r="H101" s="29" t="e">
-        <f>VLOOKUP(A101,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>1</v>
@@ -5185,13 +5501,13 @@
         <v>30</v>
       </c>
       <c r="H102" s="29" t="e">
-        <f>VLOOKUP(A102,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>2</v>
@@ -5208,7 +5524,7 @@
         <v>10</v>
       </c>
       <c r="H103" s="29" t="e">
-        <f>VLOOKUP(A103,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -5227,13 +5543,13 @@
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="29" t="e">
-        <f>VLOOKUP(A104,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B105" s="3">
         <v>48</v>
@@ -5254,13 +5570,13 @@
         <v>1620</v>
       </c>
       <c r="H105" s="29" t="e">
-        <f>VLOOKUP(A105,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B106" s="5">
         <v>48</v>
@@ -5281,13 +5597,13 @@
         <v>1024</v>
       </c>
       <c r="H106" s="29" t="e">
-        <f>VLOOKUP(A106,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B107" s="3">
         <v>96</v>
@@ -5308,13 +5624,13 @@
         <v>1400</v>
       </c>
       <c r="H107" s="29" t="e">
-        <f>VLOOKUP(A107,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B108" s="5">
         <v>144</v>
@@ -5335,13 +5651,13 @@
         <v>1440</v>
       </c>
       <c r="H108" s="29" t="e">
-        <f>VLOOKUP(A108,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B109" s="3">
         <v>144</v>
@@ -5362,13 +5678,13 @@
         <v>1740</v>
       </c>
       <c r="H109" s="29" t="e">
-        <f>VLOOKUP(A109,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B110" s="5">
         <v>192</v>
@@ -5383,19 +5699,19 @@
         <v>192</v>
       </c>
       <c r="F110" s="27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G110" s="5">
         <v>1800</v>
       </c>
       <c r="H110" s="29" t="e">
-        <f>VLOOKUP(A110,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B111" s="3">
         <v>288</v>
@@ -5416,13 +5732,13 @@
         <v>1553</v>
       </c>
       <c r="H111" s="29" t="e">
-        <f>VLOOKUP(A111,M:N,2,0)</f>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B112" s="3">
         <v>384</v>
@@ -5437,19 +5753,19 @@
         <v>320</v>
       </c>
       <c r="F112" s="26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G112" s="3">
         <v>1104</v>
       </c>
       <c r="H112" s="29" t="e">
-        <f>VLOOKUP(A112,M:N,2,0)</f>
+        <f t="shared" ref="H112:H133" si="6">ВПР(A112;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B113" s="5">
         <v>336</v>
@@ -5470,13 +5786,13 @@
         <v>16201900</v>
       </c>
       <c r="H113" s="29" t="e">
-        <f>VLOOKUP(A113,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B114" s="5">
         <v>384</v>
@@ -5497,13 +5813,13 @@
         <v>1645</v>
       </c>
       <c r="H114" s="29" t="e">
-        <f>VLOOKUP(A114,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B115" s="3">
         <v>352</v>
@@ -5524,13 +5840,13 @@
         <v>1464</v>
       </c>
       <c r="H115" s="29" t="e">
-        <f>VLOOKUP(A115,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B116" s="5">
         <v>480</v>
@@ -5551,13 +5867,13 @@
         <v>1464</v>
       </c>
       <c r="H116" s="29" t="e">
-        <f>VLOOKUP(A116,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B117" s="5">
         <v>512</v>
@@ -5578,13 +5894,13 @@
         <v>1544</v>
       </c>
       <c r="H117" s="29" t="e">
-        <f>VLOOKUP(A117,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B118" s="5">
         <v>1024</v>
@@ -5596,22 +5912,22 @@
         <v>27</v>
       </c>
       <c r="E118" s="27" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F118" s="27" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G118" s="5">
         <v>1215</v>
       </c>
       <c r="H118" s="29" t="e">
-        <f>VLOOKUP(A118,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>1</v>
@@ -5632,13 +5948,13 @@
         <v>30</v>
       </c>
       <c r="H119" s="29" t="e">
-        <f>VLOOKUP(A119,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>2</v>
@@ -5655,7 +5971,7 @@
         <v>10</v>
       </c>
       <c r="H120" s="29" t="e">
-        <f>VLOOKUP(A120,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -5674,13 +5990,13 @@
       </c>
       <c r="G121" s="4"/>
       <c r="H121" s="29" t="e">
-        <f>VLOOKUP(A121,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B122" s="3">
         <v>16</v>
@@ -5701,13 +6017,13 @@
         <v>1402</v>
       </c>
       <c r="H122" s="29" t="e">
-        <f>VLOOKUP(A122,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B123" s="3">
         <v>48</v>
@@ -5726,13 +6042,13 @@
         <v>1400</v>
       </c>
       <c r="H123" s="29" t="e">
-        <f>VLOOKUP(A123,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B124" s="5">
         <v>96</v>
@@ -5753,13 +6069,13 @@
         <v>1400</v>
       </c>
       <c r="H124" s="29" t="e">
-        <f>VLOOKUP(A124,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B125" s="5">
         <v>96</v>
@@ -5780,13 +6096,13 @@
         <v>1620</v>
       </c>
       <c r="H125" s="29" t="e">
-        <f>VLOOKUP(A125,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B126" s="5">
         <v>96</v>
@@ -5801,19 +6117,19 @@
         <v>192</v>
       </c>
       <c r="F126" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G126" s="5">
         <v>1620</v>
       </c>
       <c r="H126" s="29" t="e">
-        <f>VLOOKUP(A126,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B127" s="5">
         <v>192</v>
@@ -5828,19 +6144,19 @@
         <v>128</v>
       </c>
       <c r="F127" s="27" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G127" s="5">
         <v>1566</v>
       </c>
       <c r="H127" s="29" t="e">
-        <f>VLOOKUP(A127,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B128" s="5">
         <v>336</v>
@@ -5855,19 +6171,19 @@
         <v>256</v>
       </c>
       <c r="F128" s="27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G128" s="5">
         <v>1350</v>
       </c>
       <c r="H128" s="29" t="e">
-        <f>VLOOKUP(A128,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B129" s="5">
         <v>228</v>
@@ -5882,19 +6198,19 @@
         <v>256</v>
       </c>
       <c r="F129" s="27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G129" s="5">
         <v>1300</v>
       </c>
       <c r="H129" s="29" t="e">
-        <f>VLOOKUP(A129,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B130" s="5">
         <v>352</v>
@@ -5909,19 +6225,19 @@
         <v>256</v>
       </c>
       <c r="F130" s="27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G130" s="5">
         <v>1215</v>
       </c>
       <c r="H130" s="29" t="e">
-        <f>VLOOKUP(A130,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B131" s="5">
         <v>448</v>
@@ -5936,19 +6252,19 @@
         <v>320</v>
       </c>
       <c r="F131" s="27" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G131" s="5">
         <v>1215</v>
       </c>
       <c r="H131" s="29" t="e">
-        <f>VLOOKUP(A131,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B132" s="5">
         <v>480</v>
@@ -5963,13 +6279,13 @@
         <v>384</v>
       </c>
       <c r="F132" s="27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G132" s="5">
         <v>1401</v>
       </c>
       <c r="H132" s="29" t="e">
-        <f>VLOOKUP(A132,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -5982,7 +6298,7 @@
       <c r="F133" s="27"/>
       <c r="G133" s="5"/>
       <c r="H133" s="29" t="e">
-        <f>VLOOKUP(A133,M:N,2,0)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -6230,67 +6546,66 @@
     </row>
   </sheetData>
   <mergeCells count="173">
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="P55:P56"/>
+    <mergeCell ref="S55:S56"/>
+    <mergeCell ref="O57:O58"/>
+    <mergeCell ref="O61:O62"/>
+    <mergeCell ref="P61:P62"/>
+    <mergeCell ref="Q61:Q62"/>
+    <mergeCell ref="S61:S62"/>
+    <mergeCell ref="S59:S60"/>
+    <mergeCell ref="Q53:Q54"/>
+    <mergeCell ref="R53:R54"/>
+    <mergeCell ref="S53:S54"/>
+    <mergeCell ref="T53:T54"/>
+    <mergeCell ref="T47:T48"/>
+    <mergeCell ref="O49:O50"/>
+    <mergeCell ref="P49:P50"/>
+    <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="S49:S50"/>
+    <mergeCell ref="O51:O52"/>
+    <mergeCell ref="P51:P52"/>
+    <mergeCell ref="S51:S52"/>
+    <mergeCell ref="T31:T32"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="O33:O34"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="R33:R34"/>
+    <mergeCell ref="S33:S34"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="M35:M36"/>
+    <mergeCell ref="S45:S46"/>
+    <mergeCell ref="Q37:Q38"/>
+    <mergeCell ref="R39:R40"/>
+    <mergeCell ref="S39:S40"/>
+    <mergeCell ref="O41:O42"/>
+    <mergeCell ref="T25:T26"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="S27:S28"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="S25:S26"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="M11:M12"/>
     <mergeCell ref="S11:S12"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="M47:M48"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="M51:M52"/>
-    <mergeCell ref="M53:M54"/>
-    <mergeCell ref="M55:M56"/>
-    <mergeCell ref="P39:P40"/>
-    <mergeCell ref="Q39:Q40"/>
-    <mergeCell ref="T39:T40"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="T43:T44"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="O39:O40"/>
-    <mergeCell ref="U59:U60"/>
-    <mergeCell ref="M61:M62"/>
-    <mergeCell ref="M63:M64"/>
-    <mergeCell ref="M65:M66"/>
-    <mergeCell ref="O65:O66"/>
-    <mergeCell ref="P65:P66"/>
-    <mergeCell ref="Q65:Q66"/>
-    <mergeCell ref="T65:T66"/>
-    <mergeCell ref="M57:M58"/>
-    <mergeCell ref="M59:M60"/>
-    <mergeCell ref="O59:O60"/>
-    <mergeCell ref="P59:P60"/>
-    <mergeCell ref="Q59:Q60"/>
-    <mergeCell ref="R59:R60"/>
-    <mergeCell ref="P75:P76"/>
-    <mergeCell ref="Q75:Q76"/>
-    <mergeCell ref="S75:S76"/>
-    <mergeCell ref="M71:M72"/>
-    <mergeCell ref="Q71:Q72"/>
-    <mergeCell ref="S71:S72"/>
-    <mergeCell ref="M73:M74"/>
-    <mergeCell ref="Q73:Q74"/>
-    <mergeCell ref="M67:M68"/>
-    <mergeCell ref="P67:P68"/>
-    <mergeCell ref="Q67:Q68"/>
-    <mergeCell ref="M69:M70"/>
-    <mergeCell ref="O69:O70"/>
-    <mergeCell ref="P69:P70"/>
-    <mergeCell ref="Q69:Q70"/>
-    <mergeCell ref="S69:S70"/>
     <mergeCell ref="M81:M82"/>
     <mergeCell ref="Q81:Q82"/>
     <mergeCell ref="R81:R82"/>
@@ -6315,29 +6630,76 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="M75:M76"/>
     <mergeCell ref="O75:O76"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="T25:T26"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="S27:S28"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="P75:P76"/>
+    <mergeCell ref="Q75:Q76"/>
+    <mergeCell ref="S75:S76"/>
+    <mergeCell ref="M71:M72"/>
+    <mergeCell ref="Q71:Q72"/>
+    <mergeCell ref="S71:S72"/>
+    <mergeCell ref="M73:M74"/>
+    <mergeCell ref="Q73:Q74"/>
+    <mergeCell ref="M67:M68"/>
+    <mergeCell ref="P67:P68"/>
+    <mergeCell ref="Q67:Q68"/>
+    <mergeCell ref="M69:M70"/>
+    <mergeCell ref="O69:O70"/>
+    <mergeCell ref="P69:P70"/>
+    <mergeCell ref="Q69:Q70"/>
+    <mergeCell ref="S69:S70"/>
+    <mergeCell ref="R71:R72"/>
+    <mergeCell ref="R73:R74"/>
+    <mergeCell ref="O67:O68"/>
+    <mergeCell ref="R69:R70"/>
+    <mergeCell ref="U59:U60"/>
+    <mergeCell ref="M61:M62"/>
+    <mergeCell ref="M63:M64"/>
+    <mergeCell ref="M65:M66"/>
+    <mergeCell ref="O65:O66"/>
+    <mergeCell ref="P65:P66"/>
+    <mergeCell ref="Q65:Q66"/>
+    <mergeCell ref="T65:T66"/>
+    <mergeCell ref="M57:M58"/>
+    <mergeCell ref="M59:M60"/>
+    <mergeCell ref="O59:O60"/>
+    <mergeCell ref="P59:P60"/>
+    <mergeCell ref="Q59:Q60"/>
+    <mergeCell ref="R59:R60"/>
+    <mergeCell ref="Q63:Q64"/>
+    <mergeCell ref="S63:S64"/>
+    <mergeCell ref="R65:R66"/>
+    <mergeCell ref="S65:S66"/>
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="M53:M54"/>
+    <mergeCell ref="M55:M56"/>
+    <mergeCell ref="P39:P40"/>
+    <mergeCell ref="Q39:Q40"/>
+    <mergeCell ref="T39:T40"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="T43:T44"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="O39:O40"/>
+    <mergeCell ref="T41:T42"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="P43:P44"/>
+    <mergeCell ref="Q43:Q44"/>
+    <mergeCell ref="R43:R44"/>
+    <mergeCell ref="S43:S44"/>
+    <mergeCell ref="O47:O48"/>
+    <mergeCell ref="P47:P48"/>
+    <mergeCell ref="Q47:Q48"/>
+    <mergeCell ref="R47:R48"/>
+    <mergeCell ref="S47:S48"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="P53:P54"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="M47:M48"/>
+    <mergeCell ref="M49:M50"/>
     <mergeCell ref="S29:S30"/>
     <mergeCell ref="M31:M32"/>
     <mergeCell ref="O31:O32"/>
@@ -6345,64 +6707,18 @@
     <mergeCell ref="Q31:Q32"/>
     <mergeCell ref="R31:R32"/>
     <mergeCell ref="S31:S32"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="S25:S26"/>
     <mergeCell ref="M29:M30"/>
-    <mergeCell ref="T41:T42"/>
-    <mergeCell ref="O43:O44"/>
-    <mergeCell ref="P43:P44"/>
-    <mergeCell ref="Q43:Q44"/>
-    <mergeCell ref="R43:R44"/>
-    <mergeCell ref="S43:S44"/>
-    <mergeCell ref="T31:T32"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="O33:O34"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="R33:R34"/>
-    <mergeCell ref="S33:S34"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="M35:M36"/>
-    <mergeCell ref="S45:S46"/>
-    <mergeCell ref="O47:O48"/>
-    <mergeCell ref="P47:P48"/>
-    <mergeCell ref="Q47:Q48"/>
-    <mergeCell ref="R47:R48"/>
-    <mergeCell ref="S47:S48"/>
-    <mergeCell ref="Q37:Q38"/>
-    <mergeCell ref="R39:R40"/>
-    <mergeCell ref="S39:S40"/>
-    <mergeCell ref="O41:O42"/>
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="P53:P54"/>
-    <mergeCell ref="Q53:Q54"/>
-    <mergeCell ref="R53:R54"/>
-    <mergeCell ref="S53:S54"/>
-    <mergeCell ref="T53:T54"/>
-    <mergeCell ref="T47:T48"/>
-    <mergeCell ref="O49:O50"/>
-    <mergeCell ref="P49:P50"/>
-    <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="S49:S50"/>
-    <mergeCell ref="O51:O52"/>
-    <mergeCell ref="P51:P52"/>
-    <mergeCell ref="S51:S52"/>
-    <mergeCell ref="R71:R72"/>
-    <mergeCell ref="R73:R74"/>
-    <mergeCell ref="Q63:Q64"/>
-    <mergeCell ref="S63:S64"/>
-    <mergeCell ref="R65:R66"/>
-    <mergeCell ref="S65:S66"/>
-    <mergeCell ref="O67:O68"/>
-    <mergeCell ref="R69:R70"/>
-    <mergeCell ref="P55:P56"/>
-    <mergeCell ref="S55:S56"/>
-    <mergeCell ref="O57:O58"/>
-    <mergeCell ref="O61:O62"/>
-    <mergeCell ref="P61:P62"/>
-    <mergeCell ref="Q61:Q62"/>
-    <mergeCell ref="S61:S62"/>
-    <mergeCell ref="S59:S60"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
I DID THAT! Yeaaah! I've made this mining formula in excel
</commit_message>
<xml_diff>
--- a/bigdata/GPUs and hashrate.xlsx
+++ b/bigdata/GPUs and hashrate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ColorKat\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0613FDBF-8DA8-4B71-9851-26834AAC1F20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910C37B3-6E61-4D36-A23F-02443CBDBBEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="570" windowWidth="29040" windowHeight="15750" xr2:uid="{9B139ECC-C724-4273-A99C-4A05415BDC43}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="232">
   <si>
     <t>Memory</t>
   </si>
@@ -1269,6 +1269,41 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="2" fontId="16" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="20" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1314,41 +1349,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="5" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="20" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Акцент5" xfId="6" builtinId="45"/>
@@ -1742,7 +1742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21026847-03F0-4510-944F-5EFA55B75642}">
   <dimension ref="A1:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
@@ -1755,9 +1755,9 @@
     <col min="5" max="5" width="16.140625" style="28" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="28" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="59" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="44" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="55" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="40" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" customWidth="1"/>
     <col min="14" max="14" width="17.140625" customWidth="1"/>
@@ -1767,26 +1767,26 @@
       <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="56"/>
-      <c r="J1" s="55" t="s">
+      <c r="H1" s="41"/>
+      <c r="J1" s="40" t="s">
         <v>229</v>
       </c>
     </row>
@@ -1794,21 +1794,21 @@
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="46" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="42" t="s">
         <v>230</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -1833,32 +1833,32 @@
     </row>
     <row r="3" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="46" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="30" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="56"/>
+      <c r="H3" s="41"/>
       <c r="I3" s="29"/>
       <c r="J3"/>
-      <c r="M3" s="31" t="s">
+      <c r="M3" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="48" t="s">
         <v>95</v>
       </c>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
       <c r="T3" s="16"/>
       <c r="U3" s="10"/>
     </row>
@@ -1875,7 +1875,7 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="48">
+      <c r="E4" s="33">
         <v>128</v>
       </c>
       <c r="F4" s="27">
@@ -1884,7 +1884,7 @@
       <c r="G4" s="2">
         <v>1780</v>
       </c>
-      <c r="H4" s="58">
+      <c r="H4" s="43">
         <v>8</v>
       </c>
       <c r="I4" s="29" t="s">
@@ -1894,17 +1894,17 @@
         <f>B</f>
         <v>#NAME?</v>
       </c>
-      <c r="K4" s="55">
-        <f>КОРЕНЬ(B4) *  КОРЕНЬ(E4) * (КОРЕНЬ(F4) + 1)  * H4 ^ 0,49 / 4720,7 * 4,2</f>
-        <v>22.526576719044261</v>
-      </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="34"/>
+      <c r="K4" s="40">
+        <f xml:space="preserve"> SQRT(B4) * SQRT(E4) * IF(F4 &gt; 600, LOG(F4), SQRT(F4)) * IF(F4&lt;190, 1.1, 1) * ( SQRT(H4) * IF(H4 &lt; 5, 1.1, 1) ) / IF(F4 &gt; 600, 140, 1100) * IF(B4&lt;1300,  IF(B4&gt;1000, 1.4, 2 ), 1 )</f>
+        <v>22.029329810523663</v>
+      </c>
+      <c r="M4" s="47"/>
+      <c r="N4" s="49"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
       <c r="T4" s="17"/>
       <c r="U4" s="9"/>
     </row>
@@ -1930,19 +1930,18 @@
       <c r="G5" s="2">
         <v>1780</v>
       </c>
-      <c r="H5" s="58">
+      <c r="H5" s="43">
         <v>8</v>
       </c>
-      <c r="I5" s="29" t="str">
-        <f>ВПР(A5;M:N;2;0)</f>
-        <v>40-50MH/s*</v>
+      <c r="I5" s="29" t="s">
+        <v>201</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="55">
-        <f t="shared" ref="K5:K47" si="0">КОРЕНЬ(B5) *  КОРЕНЬ(E5) * (КОРЕНЬ(F5) + 1)  * H5 ^ 0,49 / 4720,7 * 4,2</f>
-        <v>42.108788805334278</v>
-      </c>
-      <c r="M5" s="31" t="s">
+      <c r="K5" s="40">
+        <f t="shared" ref="K5:K68" si="0" xml:space="preserve"> SQRT(B5) * SQRT(E5) * IF(F5 &gt; 600, LOG(F5), SQRT(F5)) * IF(F5&lt;190, 1.1, 1) * ( SQRT(H5) * IF(H5 &lt; 5, 1.1, 1) ) / IF(F5 &gt; 600, 140, 1100) * IF(B5&lt;1300,  IF(B5&gt;1000, 1.4, 2 ), 1 )</f>
+        <v>41.797714516980172</v>
+      </c>
+      <c r="M5" s="46" t="s">
         <v>223</v>
       </c>
       <c r="N5" s="16" t="s">
@@ -1950,7 +1949,7 @@
       </c>
       <c r="O5" s="16"/>
       <c r="P5" s="16"/>
-      <c r="Q5" s="33"/>
+      <c r="Q5" s="48"/>
       <c r="R5" s="16"/>
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
@@ -1960,7 +1959,7 @@
       <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="36">
         <v>4864</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1969,7 +1968,7 @@
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="39">
         <v>256</v>
       </c>
       <c r="F6" s="27">
@@ -1978,27 +1977,26 @@
       <c r="G6" s="2">
         <v>1670</v>
       </c>
-      <c r="H6" s="58">
+      <c r="H6" s="43">
         <v>8</v>
       </c>
-      <c r="I6" s="29" t="str">
-        <f>ВПР(A6;M:N;2;0)</f>
-        <v>55-63Mh/s</v>
+      <c r="I6" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="J6">
         <v>60.2</v>
       </c>
-      <c r="K6" s="55">
+      <c r="K6" s="40">
         <f t="shared" si="0"/>
-        <v>60.962291362575471</v>
-      </c>
-      <c r="M6" s="32"/>
+        <v>60.730671216826543</v>
+      </c>
+      <c r="M6" s="47"/>
       <c r="N6" s="17" t="s">
         <v>34</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="34"/>
+      <c r="Q6" s="49"/>
       <c r="R6" s="17"/>
       <c r="S6" s="17"/>
       <c r="T6" s="17"/>
@@ -2008,7 +2006,7 @@
       <c r="A7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="36">
         <v>5888</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2017,38 +2015,37 @@
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="39">
         <v>256</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="34">
         <v>448</v>
       </c>
       <c r="G7" s="2">
         <v>1770</v>
       </c>
-      <c r="H7" s="58">
+      <c r="H7" s="43">
         <v>8</v>
       </c>
-      <c r="I7" s="29" t="str">
-        <f>ВПР(A7;M:N;2;0)</f>
-        <v>55-63MH/s</v>
+      <c r="I7" s="29" t="s">
+        <v>71</v>
       </c>
       <c r="J7">
         <v>61.7</v>
       </c>
-      <c r="K7" s="55">
+      <c r="K7" s="40">
         <f t="shared" si="0"/>
-        <v>67.073103193470729</v>
-      </c>
-      <c r="M7" s="31" t="s">
+        <v>66.818265627653076</v>
+      </c>
+      <c r="M7" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N7" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
       <c r="R7" s="16"/>
       <c r="S7" s="16"/>
       <c r="T7" s="16"/>
@@ -2067,34 +2064,33 @@
       <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="39">
         <v>256</v>
       </c>
-      <c r="F8" s="49">
+      <c r="F8" s="34">
         <v>608</v>
       </c>
       <c r="G8" s="2">
         <v>1730</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="43">
         <v>8</v>
       </c>
-      <c r="I8" s="29" t="str">
-        <f>ВПР(A8;M:N;2;0)</f>
-        <v>80Mh/s*</v>
+      <c r="I8" s="29" t="s">
+        <v>115</v>
       </c>
       <c r="J8">
         <v>81.8</v>
       </c>
-      <c r="K8" s="55">
+      <c r="K8" s="40">
         <f t="shared" si="0"/>
-        <v>79.308465420131682</v>
-      </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
+        <v>70.536959161391238</v>
+      </c>
+      <c r="M8" s="47"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17"/>
@@ -2122,19 +2118,18 @@
       <c r="G9" s="2">
         <v>1710</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="43">
         <v>10</v>
       </c>
-      <c r="I9" s="29" t="str">
-        <f>ВПР(A9;M:N;2;0)</f>
-        <v>95-105Mh/s</v>
+      <c r="I9" s="29" t="s">
+        <v>76</v>
       </c>
       <c r="J9"/>
-      <c r="K9" s="55">
+      <c r="K9" s="40">
         <f t="shared" si="0"/>
-        <v>131.08670231068592</v>
-      </c>
-      <c r="M9" s="31" t="s">
+        <v>108.59793123372575</v>
+      </c>
+      <c r="M9" s="46" t="s">
         <v>36</v>
       </c>
       <c r="N9" s="16" t="s">
@@ -2143,7 +2138,7 @@
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
-      <c r="R9" s="33"/>
+      <c r="R9" s="48"/>
       <c r="S9" s="16"/>
       <c r="T9" s="16"/>
       <c r="U9" s="10"/>
@@ -2164,34 +2159,33 @@
       <c r="E10" s="25">
         <v>384</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="34">
         <v>912</v>
       </c>
       <c r="G10" s="2">
         <v>1670</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="43">
         <v>12</v>
       </c>
-      <c r="I10" s="29" t="str">
-        <f>ВПР(A10;M:N;2;0)</f>
-        <v>112Mh/s*</v>
+      <c r="I10" s="29" t="s">
+        <v>224</v>
       </c>
       <c r="J10">
         <v>112</v>
       </c>
-      <c r="K10" s="55">
+      <c r="K10" s="40">
         <f t="shared" si="0"/>
-        <v>185.9955976622623</v>
-      </c>
-      <c r="M10" s="32"/>
+        <v>145.23427850717266</v>
+      </c>
+      <c r="M10" s="47"/>
       <c r="N10" s="17" t="s">
         <v>35</v>
       </c>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
-      <c r="R10" s="34"/>
+      <c r="R10" s="49"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="9"/>
@@ -2212,27 +2206,26 @@
       <c r="E11" s="25">
         <v>384</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="34">
         <v>936</v>
       </c>
       <c r="G11" s="2">
         <v>1700</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H11" s="43">
         <v>24</v>
       </c>
-      <c r="I11" s="29" t="str">
-        <f>ВПР(A11;M:N;2;0)</f>
-        <v>100-122Mh/s</v>
+      <c r="I11" s="29" t="s">
+        <v>82</v>
       </c>
       <c r="J11">
         <v>121</v>
       </c>
-      <c r="K11" s="55">
+      <c r="K11" s="40">
         <f t="shared" si="0"/>
-        <v>267.81206816380876</v>
-      </c>
-      <c r="M11" s="31" t="s">
+        <v>208.73634819460185</v>
+      </c>
+      <c r="M11" s="46" t="s">
         <v>103</v>
       </c>
       <c r="N11" s="16" t="s">
@@ -2242,8 +2235,8 @@
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="35"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="50"/>
       <c r="U11" s="10"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2259,7 +2252,7 @@
       <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="33">
         <v>256</v>
       </c>
       <c r="F12" s="27">
@@ -2268,18 +2261,18 @@
       <c r="G12" s="5">
         <v>1244</v>
       </c>
-      <c r="H12" s="58">
+      <c r="H12" s="43">
         <v>8</v>
       </c>
       <c r="I12" s="29" t="s">
         <v>64</v>
       </c>
       <c r="J12"/>
-      <c r="K12" s="55">
+      <c r="K12" s="40">
         <f t="shared" si="0"/>
-        <v>28.494116127481107</v>
-      </c>
-      <c r="M12" s="32"/>
+        <v>27.865143011320118</v>
+      </c>
+      <c r="M12" s="47"/>
       <c r="N12" s="23" t="s">
         <v>38</v>
       </c>
@@ -2287,8 +2280,8 @@
       <c r="P12" s="23"/>
       <c r="Q12" s="23"/>
       <c r="R12" s="23"/>
-      <c r="S12" s="34"/>
-      <c r="T12" s="36"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="51"/>
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2298,10 +2291,10 @@
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="45" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="24" t="s">
@@ -2313,17 +2306,16 @@
       <c r="G13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="56"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="29" t="e">
-        <f>ВПР(A13;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J13"/>
-      <c r="K13" s="55" t="e">
+      <c r="K13" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M13" s="31" t="s">
+      <c r="M13" s="46" t="s">
         <v>104</v>
       </c>
       <c r="N13" s="16" t="s">
@@ -2344,8 +2336,8 @@
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="24" t="s">
         <v>6</v>
       </c>
@@ -2355,19 +2347,18 @@
       <c r="G14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="57" t="s">
+      <c r="H14" s="42" t="s">
         <v>230</v>
       </c>
       <c r="I14" s="29" t="e">
-        <f>ВПР(A14;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J14"/>
-      <c r="K14" s="55" t="e">
+      <c r="K14" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M14" s="32"/>
+      <c r="M14" s="47"/>
       <c r="N14" s="17" t="s">
         <v>41</v>
       </c>
@@ -2384,8 +2375,8 @@
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="24" t="s">
         <v>7</v>
       </c>
@@ -2393,28 +2384,27 @@
         <v>9</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="56"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="29" t="e">
-        <f>ВПР(A15;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J15"/>
-      <c r="K15" s="55" t="e">
+      <c r="K15" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M15" s="31" t="s">
+      <c r="M15" s="46" t="s">
         <v>43</v>
       </c>
       <c r="N15" s="16" t="s">
         <v>44</v>
       </c>
       <c r="O15" s="16"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="35"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="50"/>
       <c r="U15" s="10"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2439,35 +2429,34 @@
       <c r="G16" s="2">
         <v>1680</v>
       </c>
-      <c r="H16" s="58">
+      <c r="H16" s="43">
         <v>6</v>
       </c>
-      <c r="I16" s="29" t="str">
-        <f>ВПР(A16;M:N;2;0)</f>
-        <v>25-30Mh/s</v>
+      <c r="I16" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="J16"/>
-      <c r="K16" s="55">
+      <c r="K16" s="40">
         <f t="shared" si="0"/>
-        <v>25.123311694714221</v>
-      </c>
-      <c r="M16" s="32"/>
+        <v>24.782996036839116</v>
+      </c>
+      <c r="M16" s="47"/>
       <c r="N16" s="17" t="s">
         <v>45</v>
       </c>
       <c r="O16" s="17"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="36"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="51"/>
       <c r="U16" s="9"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="51">
+      <c r="B17" s="36">
         <v>2176</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -2476,7 +2465,7 @@
       <c r="D17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="39">
         <v>256</v>
       </c>
       <c r="F17" s="27">
@@ -2485,21 +2474,20 @@
       <c r="G17" s="2">
         <v>1650</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="43">
         <v>8</v>
       </c>
-      <c r="I17" s="29" t="str">
-        <f>ВПР(A17;M:N;2;0)</f>
-        <v> 36-42 Mh/s</v>
+      <c r="I17" s="29" t="s">
+        <v>56</v>
       </c>
       <c r="J17">
         <v>38.700000000000003</v>
       </c>
-      <c r="K17" s="55">
+      <c r="K17" s="40">
         <f t="shared" si="0"/>
-        <v>40.774997647224517</v>
-      </c>
-      <c r="M17" s="31" t="s">
+        <v>40.62007711049808</v>
+      </c>
+      <c r="M17" s="46" t="s">
         <v>49</v>
       </c>
       <c r="N17" s="16" t="s">
@@ -2507,7 +2495,7 @@
       </c>
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
-      <c r="Q17" s="33"/>
+      <c r="Q17" s="48"/>
       <c r="R17" s="16"/>
       <c r="S17" s="16"/>
       <c r="T17" s="16"/>
@@ -2526,7 +2514,7 @@
       <c r="D18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="39">
         <v>256</v>
       </c>
       <c r="F18" s="27">
@@ -2535,27 +2523,26 @@
       <c r="G18" s="2">
         <v>1620</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="43">
         <v>8</v>
       </c>
-      <c r="I18" s="29" t="str">
-        <f>ВПР(A18;M:N;2;0)</f>
-        <v> 36-42Mh/s</v>
+      <c r="I18" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="J18">
         <v>39.799999999999997</v>
       </c>
-      <c r="K18" s="55">
+      <c r="K18" s="40">
         <f t="shared" si="0"/>
-        <v>41.957126434128782</v>
-      </c>
-      <c r="M18" s="32"/>
+        <v>41.797714516980179</v>
+      </c>
+      <c r="M18" s="47"/>
       <c r="N18" s="17" t="s">
         <v>34</v>
       </c>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="34"/>
+      <c r="Q18" s="49"/>
       <c r="R18" s="17"/>
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
@@ -2583,31 +2570,30 @@
       <c r="G19" s="2">
         <v>1770</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="43">
         <v>8</v>
       </c>
-      <c r="I19" s="29" t="str">
-        <f>ВПР(A19;M:N;2;0)</f>
-        <v> 36-42Mh/s</v>
+      <c r="I19" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="J19">
         <v>46</v>
       </c>
-      <c r="K19" s="55">
+      <c r="K19" s="40">
         <f t="shared" si="0"/>
-        <v>44.2266945358352</v>
-      </c>
-      <c r="M19" s="31" t="s">
+        <v>44.058659621047326</v>
+      </c>
+      <c r="M19" s="46" t="s">
         <v>51</v>
       </c>
       <c r="N19" s="16" t="s">
         <v>52</v>
       </c>
       <c r="O19" s="16"/>
-      <c r="P19" s="33"/>
+      <c r="P19" s="48"/>
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
-      <c r="S19" s="33"/>
+      <c r="S19" s="48"/>
       <c r="T19" s="16"/>
       <c r="U19" s="10"/>
     </row>
@@ -2615,7 +2601,7 @@
       <c r="A20" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B20" s="51">
+      <c r="B20" s="36">
         <v>2944</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -2633,29 +2619,28 @@
       <c r="G20" s="2">
         <v>1710</v>
       </c>
-      <c r="H20" s="58">
+      <c r="H20" s="43">
         <v>8</v>
       </c>
-      <c r="I20" s="29" t="str">
-        <f>ВПР(A20;M:N;2;0)</f>
-        <v>36-44Mh/s</v>
+      <c r="I20" s="29" t="s">
+        <v>60</v>
       </c>
       <c r="J20">
         <v>47</v>
       </c>
-      <c r="K20" s="55">
+      <c r="K20" s="40">
         <f t="shared" si="0"/>
-        <v>47.427846103328228</v>
-      </c>
-      <c r="M20" s="32"/>
+        <v>47.24764873243749</v>
+      </c>
+      <c r="M20" s="47"/>
       <c r="N20" s="17" t="s">
         <v>48</v>
       </c>
       <c r="O20" s="17"/>
-      <c r="P20" s="34"/>
+      <c r="P20" s="49"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
-      <c r="S20" s="34"/>
+      <c r="S20" s="49"/>
       <c r="T20" s="17"/>
       <c r="U20" s="9"/>
     </row>
@@ -2681,19 +2666,18 @@
       <c r="G21" s="2">
         <v>1815</v>
       </c>
-      <c r="H21" s="58">
+      <c r="H21" s="43">
         <v>8</v>
       </c>
-      <c r="I21" s="29" t="str">
-        <f>ВПР(A21;M:N;2;0)</f>
-        <v>36-44Mh/s</v>
+      <c r="I21" s="29" t="s">
+        <v>60</v>
       </c>
       <c r="J21"/>
-      <c r="K21" s="55">
+      <c r="K21" s="40">
         <f t="shared" si="0"/>
-        <v>50.863201045639094</v>
-      </c>
-      <c r="M21" s="31" t="s">
+        <v>50.783629300776411</v>
+      </c>
+      <c r="M21" s="46" t="s">
         <v>53</v>
       </c>
       <c r="N21" s="16" t="s">
@@ -2701,7 +2685,7 @@
       </c>
       <c r="O21" s="16"/>
       <c r="P21" s="16"/>
-      <c r="Q21" s="33"/>
+      <c r="Q21" s="48"/>
       <c r="R21" s="16"/>
       <c r="S21" s="16"/>
       <c r="T21" s="16"/>
@@ -2729,25 +2713,24 @@
       <c r="G22" s="2">
         <v>1545</v>
       </c>
-      <c r="H22" s="58">
+      <c r="H22" s="43">
         <v>11</v>
       </c>
-      <c r="I22" s="29" t="str">
-        <f>ВПР(A22;M:N;2;0)</f>
-        <v>50-57Mh/s</v>
+      <c r="I22" s="29" t="s">
+        <v>113</v>
       </c>
       <c r="J22"/>
-      <c r="K22" s="55">
+      <c r="K22" s="40">
         <f t="shared" si="0"/>
-        <v>92.063257684048082</v>
-      </c>
-      <c r="M22" s="32"/>
+        <v>81.794295009650128</v>
+      </c>
+      <c r="M22" s="47"/>
       <c r="N22" s="17" t="s">
         <v>55</v>
       </c>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="34"/>
+      <c r="Q22" s="49"/>
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
       <c r="T22" s="17"/>
@@ -2775,18 +2758,18 @@
       <c r="G23" s="2">
         <v>1770</v>
       </c>
-      <c r="H23" s="58">
+      <c r="H23" s="43">
         <v>24</v>
       </c>
       <c r="I23" s="29" t="s">
         <v>228</v>
       </c>
       <c r="J23"/>
-      <c r="K23" s="55">
+      <c r="K23" s="40">
         <f t="shared" si="0"/>
-        <v>151.2136843926624</v>
-      </c>
-      <c r="M23" s="31" t="s">
+        <v>131.60790215719166</v>
+      </c>
+      <c r="M23" s="46" t="s">
         <v>106</v>
       </c>
       <c r="N23" s="16" t="s">
@@ -2794,7 +2777,7 @@
       </c>
       <c r="O23" s="16"/>
       <c r="P23" s="16"/>
-      <c r="Q23" s="33"/>
+      <c r="Q23" s="48"/>
       <c r="R23" s="16"/>
       <c r="S23" s="16"/>
       <c r="T23" s="16"/>
@@ -2808,23 +2791,22 @@
       <c r="E24" s="25"/>
       <c r="F24" s="27"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="58"/>
+      <c r="H24" s="43"/>
       <c r="I24" s="29" t="e">
-        <f>ВПР(A24;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J24"/>
-      <c r="K24" s="55">
+      <c r="K24" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M24" s="32"/>
+      <c r="M24" s="47"/>
       <c r="N24" s="17" t="s">
         <v>35</v>
       </c>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="34"/>
+      <c r="Q24" s="49"/>
       <c r="R24" s="17"/>
       <c r="S24" s="17"/>
       <c r="T24" s="17"/>
@@ -2837,10 +2819,10 @@
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="45" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2852,28 +2834,27 @@
       <c r="G25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="56"/>
+      <c r="H25" s="41"/>
       <c r="I25" s="29" t="e">
-        <f>ВПР(A25;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J25"/>
-      <c r="K25" s="55" t="e">
+      <c r="K25" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M25" s="31" t="s">
+      <c r="M25" s="46" t="s">
         <v>108</v>
       </c>
       <c r="N25" s="16" t="s">
         <v>56</v>
       </c>
       <c r="O25" s="16"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="48"/>
       <c r="R25" s="16"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="35"/>
+      <c r="S25" s="48"/>
+      <c r="T25" s="50"/>
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2883,8 +2864,8 @@
       <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="24" t="s">
         <v>6</v>
       </c>
@@ -2894,28 +2875,27 @@
       <c r="G26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="57" t="s">
+      <c r="H26" s="42" t="s">
         <v>230</v>
       </c>
       <c r="I26" s="29" t="e">
-        <f>ВПР(A26;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J26"/>
-      <c r="K26" s="55" t="e">
+      <c r="K26" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M26" s="32"/>
+      <c r="M26" s="47"/>
       <c r="N26" s="17" t="s">
         <v>57</v>
       </c>
       <c r="O26" s="17"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
       <c r="R26" s="17"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="36"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="51"/>
       <c r="U26" s="9"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2923,8 +2903,8 @@
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
       <c r="E27" s="24" t="s">
         <v>7</v>
       </c>
@@ -2932,17 +2912,16 @@
         <v>9</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="56"/>
+      <c r="H27" s="41"/>
       <c r="I27" s="29" t="e">
-        <f>ВПР(A27;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J27"/>
-      <c r="K27" s="55" t="e">
+      <c r="K27" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M27" s="31" t="s">
+      <c r="M27" s="46" t="s">
         <v>109</v>
       </c>
       <c r="N27" s="16" t="s">
@@ -2952,7 +2931,7 @@
       <c r="P27" s="16"/>
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
-      <c r="S27" s="33"/>
+      <c r="S27" s="48"/>
       <c r="T27" s="16"/>
       <c r="U27" s="10"/>
     </row>
@@ -2978,19 +2957,18 @@
       <c r="G28" s="2">
         <v>1665</v>
       </c>
-      <c r="H28" s="58">
+      <c r="H28" s="43">
         <v>4</v>
       </c>
-      <c r="I28" s="29" t="str">
-        <f>ВПР(A28;M:N;2;0)</f>
-        <v> 14-16MH/s</v>
+      <c r="I28" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="J28"/>
-      <c r="K28" s="55">
+      <c r="K28" s="40">
         <f t="shared" si="0"/>
-        <v>7.3181303735523038</v>
-      </c>
-      <c r="M28" s="32"/>
+        <v>16.858411521848673</v>
+      </c>
+      <c r="M28" s="47"/>
       <c r="N28" s="17" t="s">
         <v>39</v>
       </c>
@@ -2998,7 +2976,7 @@
       <c r="P28" s="17"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
-      <c r="S28" s="34"/>
+      <c r="S28" s="49"/>
       <c r="T28" s="17"/>
       <c r="U28" s="9"/>
     </row>
@@ -3024,18 +3002,18 @@
       <c r="G29" s="2">
         <v>1725</v>
       </c>
-      <c r="H29" s="58">
+      <c r="H29" s="43">
         <v>4</v>
       </c>
       <c r="I29" s="29" t="s">
         <v>227</v>
       </c>
       <c r="J29"/>
-      <c r="K29" s="55">
+      <c r="K29" s="40">
         <f t="shared" si="0"/>
-        <v>10.553002152811878</v>
-      </c>
-      <c r="M29" s="31" t="s">
+        <v>15.704301168788124</v>
+      </c>
+      <c r="M29" s="46" t="s">
         <v>110</v>
       </c>
       <c r="N29" s="16" t="s">
@@ -3045,7 +3023,7 @@
       <c r="P29" s="16"/>
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
-      <c r="S29" s="33"/>
+      <c r="S29" s="48"/>
       <c r="T29" s="16"/>
       <c r="U29" s="10"/>
     </row>
@@ -3065,25 +3043,24 @@
       <c r="E30" s="25">
         <v>192</v>
       </c>
-      <c r="F30" s="50">
+      <c r="F30" s="35">
         <v>192</v>
       </c>
       <c r="G30" s="2">
         <v>1785</v>
       </c>
-      <c r="H30" s="58">
+      <c r="H30" s="43">
         <v>6</v>
       </c>
-      <c r="I30" s="29" t="str">
-        <f>ВПР(A30;M:N;2;0)</f>
-        <v> 20-25Mh/s</v>
+      <c r="I30" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="J30"/>
-      <c r="K30" s="55">
+      <c r="K30" s="40">
         <f t="shared" si="0"/>
-        <v>16.534943519585678</v>
-      </c>
-      <c r="M30" s="32"/>
+        <v>16.04299677287711</v>
+      </c>
+      <c r="M30" s="47"/>
       <c r="N30" s="17" t="s">
         <v>39</v>
       </c>
@@ -3091,7 +3068,7 @@
       <c r="P30" s="17"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="17"/>
-      <c r="S30" s="34"/>
+      <c r="S30" s="49"/>
       <c r="T30" s="17"/>
       <c r="U30" s="9"/>
     </row>
@@ -3111,36 +3088,35 @@
       <c r="E31" s="25">
         <v>192</v>
       </c>
-      <c r="F31" s="50">
+      <c r="F31" s="35">
         <v>336</v>
       </c>
       <c r="G31" s="2">
         <v>1785</v>
       </c>
-      <c r="H31" s="58">
+      <c r="H31" s="43">
         <v>6</v>
       </c>
-      <c r="I31" s="29" t="str">
-        <f>ВПР(A31;M:N;2;0)</f>
-        <v>25-31Mh/s</v>
+      <c r="I31" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="J31"/>
-      <c r="K31" s="55">
+      <c r="K31" s="40">
         <f t="shared" si="0"/>
-        <v>21.514318790993453</v>
-      </c>
-      <c r="M31" s="31" t="s">
+        <v>21.222889872622307</v>
+      </c>
+      <c r="M31" s="46" t="s">
         <v>111</v>
       </c>
       <c r="N31" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="33"/>
-      <c r="S31" s="33"/>
-      <c r="T31" s="35"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="50"/>
       <c r="U31" s="10"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3159,34 +3135,33 @@
       <c r="E32" s="25">
         <v>192</v>
       </c>
-      <c r="F32" s="49">
+      <c r="F32" s="34">
         <v>288</v>
       </c>
       <c r="G32" s="2">
         <v>1770</v>
       </c>
-      <c r="H32" s="58">
+      <c r="H32" s="43">
         <v>6</v>
       </c>
-      <c r="I32" s="29" t="str">
-        <f>ВПР(A32;M:N;2;0)</f>
-        <v> 24-31,5Mh/s</v>
+      <c r="I32" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="J32"/>
-      <c r="K32" s="55">
+      <c r="K32" s="40">
         <f t="shared" si="0"/>
-        <v>20.890310764976494</v>
-      </c>
-      <c r="M32" s="32"/>
+        <v>20.522270426808877</v>
+      </c>
+      <c r="M32" s="47"/>
       <c r="N32" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="O32" s="34"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="34"/>
-      <c r="T32" s="36"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="51"/>
       <c r="U32" s="9"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3197,27 +3172,26 @@
       <c r="E33" s="25"/>
       <c r="F33" s="27"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="58"/>
+      <c r="H33" s="43"/>
       <c r="I33" s="29" t="e">
-        <f>ВПР(A33;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J33"/>
-      <c r="K33" s="55">
+      <c r="K33" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M33" s="31" t="s">
+      <c r="M33" s="46" t="s">
         <v>61</v>
       </c>
       <c r="N33" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
+      <c r="O33" s="48"/>
+      <c r="P33" s="48"/>
       <c r="Q33" s="16"/>
-      <c r="R33" s="33"/>
-      <c r="S33" s="33"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="48"/>
       <c r="T33" s="16"/>
       <c r="U33" s="10"/>
     </row>
@@ -3228,10 +3202,10 @@
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="45" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="24" t="s">
@@ -3243,25 +3217,24 @@
       <c r="G34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="56"/>
+      <c r="H34" s="41"/>
       <c r="I34" s="29" t="e">
-        <f>ВПР(A34;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J34"/>
-      <c r="K34" s="55" t="e">
+      <c r="K34" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M34" s="32"/>
+      <c r="M34" s="47"/>
       <c r="N34" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="O34" s="34"/>
-      <c r="P34" s="34"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
       <c r="Q34" s="17"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="34"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
       <c r="T34" s="17"/>
       <c r="U34" s="11"/>
     </row>
@@ -3272,8 +3245,8 @@
       <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
       <c r="E35" s="24" t="s">
         <v>6</v>
       </c>
@@ -3283,19 +3256,18 @@
       <c r="G35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H35" s="57" t="s">
+      <c r="H35" s="42" t="s">
         <v>230</v>
       </c>
       <c r="I35" s="29" t="e">
-        <f>ВПР(A35;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J35"/>
-      <c r="K35" s="55" t="e">
+      <c r="K35" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M35" s="31" t="s">
+      <c r="M35" s="46" t="s">
         <v>112</v>
       </c>
       <c r="N35" s="16" t="s">
@@ -3314,8 +3286,8 @@
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="24" t="s">
         <v>7</v>
       </c>
@@ -3323,17 +3295,16 @@
         <v>9</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="56"/>
+      <c r="H36" s="41"/>
       <c r="I36" s="29" t="e">
-        <f>ВПР(A36;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J36"/>
-      <c r="K36" s="55" t="e">
+      <c r="K36" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M36" s="32"/>
+      <c r="M36" s="47"/>
       <c r="N36" s="17" t="s">
         <v>63</v>
       </c>
@@ -3367,17 +3338,16 @@
       <c r="G37" s="2">
         <v>1468</v>
       </c>
-      <c r="H37" s="58"/>
+      <c r="H37" s="43"/>
       <c r="I37" s="29" t="e">
-        <f>ВПР(A37;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J37"/>
-      <c r="K37" s="55" t="e">
+      <c r="K37" s="40" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M37" s="31" t="s">
+      <c r="M37" s="46" t="s">
         <v>65</v>
       </c>
       <c r="N37" s="16" t="s">
@@ -3385,7 +3355,7 @@
       </c>
       <c r="O37" s="16"/>
       <c r="P37" s="16"/>
-      <c r="Q37" s="33"/>
+      <c r="Q37" s="48"/>
       <c r="R37" s="16"/>
       <c r="S37" s="16"/>
       <c r="T37" s="16"/>
@@ -3413,24 +3383,24 @@
       <c r="G38" s="2">
         <v>1468</v>
       </c>
-      <c r="H38" s="58">
+      <c r="H38" s="43">
         <v>2</v>
       </c>
-      <c r="I38" s="53"/>
+      <c r="I38" s="38"/>
       <c r="J38">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K38" s="55">
+      <c r="K38" s="40">
         <f t="shared" si="0"/>
-        <v>1.5530232580522259</v>
-      </c>
-      <c r="M38" s="32"/>
+        <v>3.3792000000000004</v>
+      </c>
+      <c r="M38" s="47"/>
       <c r="N38" s="17" t="s">
         <v>35</v>
       </c>
       <c r="O38" s="17"/>
       <c r="P38" s="17"/>
-      <c r="Q38" s="34"/>
+      <c r="Q38" s="49"/>
       <c r="R38" s="17"/>
       <c r="S38" s="17"/>
       <c r="T38" s="17"/>
@@ -3458,30 +3428,29 @@
       <c r="G39" s="2">
         <v>1455</v>
       </c>
-      <c r="H39" s="58">
+      <c r="H39" s="43">
         <v>2</v>
       </c>
       <c r="I39" s="29" t="e">
-        <f>ВПР(A39;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J39"/>
-      <c r="K39" s="55">
+      <c r="K39" s="40">
         <f t="shared" si="0"/>
-        <v>4.1425123430876614</v>
-      </c>
-      <c r="M39" s="31" t="s">
+        <v>9.4241385388798324</v>
+      </c>
+      <c r="M39" s="46" t="s">
         <v>66</v>
       </c>
       <c r="N39" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33"/>
-      <c r="Q39" s="33"/>
-      <c r="R39" s="33"/>
-      <c r="S39" s="33"/>
-      <c r="T39" s="35"/>
+      <c r="O39" s="48"/>
+      <c r="P39" s="48"/>
+      <c r="Q39" s="48"/>
+      <c r="R39" s="48"/>
+      <c r="S39" s="48"/>
+      <c r="T39" s="50"/>
       <c r="U39" s="9"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3506,28 +3475,27 @@
       <c r="G40" s="2">
         <v>1518</v>
       </c>
-      <c r="H40" s="58">
+      <c r="H40" s="43">
         <v>3</v>
       </c>
       <c r="I40" s="29" t="e">
-        <f>ВПР(A40;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J40"/>
-      <c r="K40" s="55">
+      <c r="K40" s="40">
         <f t="shared" si="0"/>
-        <v>4.2069018602055435</v>
-      </c>
-      <c r="M40" s="32"/>
+        <v>9.4828564810398763</v>
+      </c>
+      <c r="M40" s="47"/>
       <c r="N40" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="O40" s="34"/>
-      <c r="P40" s="34"/>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="34"/>
-      <c r="S40" s="34"/>
-      <c r="T40" s="36"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="51"/>
       <c r="U40" s="10"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -3552,30 +3520,29 @@
       <c r="G41" s="2">
         <v>1392</v>
       </c>
-      <c r="H41" s="58">
+      <c r="H41" s="43">
         <v>4</v>
       </c>
-      <c r="I41" s="29" t="str">
-        <f>ВПР(A41;M:N;2;0)</f>
-        <v>15Mh/s</v>
+      <c r="I41" s="29" t="s">
+        <v>95</v>
       </c>
       <c r="J41"/>
-      <c r="K41" s="55">
+      <c r="K41" s="40">
         <f t="shared" si="0"/>
-        <v>6.3732232531350457</v>
-      </c>
-      <c r="M41" s="31" t="s">
+        <v>14.599812645373232</v>
+      </c>
+      <c r="M41" s="46" t="s">
         <v>67</v>
       </c>
       <c r="N41" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="O41" s="33"/>
+      <c r="O41" s="48"/>
       <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
       <c r="S41" s="16"/>
-      <c r="T41" s="35"/>
+      <c r="T41" s="50"/>
       <c r="U41" s="9"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3600,27 +3567,27 @@
       <c r="G42" s="2">
         <v>1708</v>
       </c>
-      <c r="H42" s="58">
+      <c r="H42" s="43">
         <v>3</v>
       </c>
       <c r="I42" s="29" t="s">
         <v>231</v>
       </c>
       <c r="J42"/>
-      <c r="K42" s="55">
+      <c r="K42" s="40">
         <f t="shared" si="0"/>
-        <v>10.649345814632834</v>
-      </c>
-      <c r="M42" s="32"/>
+        <v>15.802148228642835</v>
+      </c>
+      <c r="M42" s="47"/>
       <c r="N42" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="O42" s="34"/>
+      <c r="O42" s="49"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="17"/>
       <c r="R42" s="17"/>
       <c r="S42" s="17"/>
-      <c r="T42" s="36"/>
+      <c r="T42" s="51"/>
       <c r="U42" s="10"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -3645,37 +3612,36 @@
       <c r="G43" s="2">
         <v>1708</v>
       </c>
-      <c r="H43" s="58">
+      <c r="H43" s="43">
         <v>6</v>
       </c>
-      <c r="I43" s="29" t="str">
-        <f>ВПР(A43;M:N;2;0)</f>
-        <v>17-23Mh/s</v>
+      <c r="I43" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="J43"/>
-      <c r="K43" s="55">
+      <c r="K43" s="40">
         <f t="shared" si="0"/>
-        <v>15.765450061213784</v>
-      </c>
-      <c r="M43" s="31" t="s">
+        <v>21.414956139256525</v>
+      </c>
+      <c r="M43" s="46" t="s">
         <v>69</v>
       </c>
       <c r="N43" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="O43" s="33"/>
-      <c r="P43" s="33"/>
-      <c r="Q43" s="33"/>
-      <c r="R43" s="33"/>
-      <c r="S43" s="33"/>
-      <c r="T43" s="35"/>
+      <c r="O43" s="48"/>
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="50"/>
       <c r="U43" s="9"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="52">
+      <c r="B44" s="37">
         <v>1920</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -3693,35 +3659,34 @@
       <c r="G44" s="2">
         <v>1683</v>
       </c>
-      <c r="H44" s="58">
+      <c r="H44" s="43">
         <v>8</v>
       </c>
-      <c r="I44" s="29" t="str">
-        <f>ВПР(A44;M:N;2;0)</f>
-        <v> 24-28Mh/s120W</v>
+      <c r="I44" s="29" t="s">
+        <v>102</v>
       </c>
       <c r="J44"/>
-      <c r="K44" s="55">
-        <f t="shared" si="0"/>
-        <v>29.374907010259292</v>
-      </c>
-      <c r="M44" s="32"/>
+      <c r="K44" s="40" t="e">
+        <f>K25</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M44" s="47"/>
       <c r="N44" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="O44" s="34"/>
-      <c r="P44" s="34"/>
-      <c r="Q44" s="34"/>
-      <c r="R44" s="34"/>
-      <c r="S44" s="34"/>
-      <c r="T44" s="36"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="49"/>
+      <c r="T44" s="51"/>
       <c r="U44" s="10"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="52">
+      <c r="B45" s="37">
         <v>2432</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -3733,25 +3698,24 @@
       <c r="E45" s="25">
         <v>256</v>
       </c>
-      <c r="F45" s="49">
+      <c r="F45" s="34">
         <v>256</v>
       </c>
       <c r="G45" s="2">
         <v>1683</v>
       </c>
-      <c r="H45" s="58">
+      <c r="H45" s="43">
         <v>8</v>
       </c>
-      <c r="I45" s="29" t="str">
-        <f>ВПР(A45;M:N;2;0)</f>
-        <v> 25-29Mh/s</v>
+      <c r="I45" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="J45"/>
-      <c r="K45" s="55">
+      <c r="K45" s="40">
         <f t="shared" si="0"/>
-        <v>33.060367083429099</v>
-      </c>
-      <c r="M45" s="31" t="s">
+        <v>32.461909223168362</v>
+      </c>
+      <c r="M45" s="46" t="s">
         <v>70</v>
       </c>
       <c r="N45" s="16" t="s">
@@ -3761,7 +3725,7 @@
       <c r="P45" s="16"/>
       <c r="Q45" s="16"/>
       <c r="R45" s="16"/>
-      <c r="S45" s="33"/>
+      <c r="S45" s="48"/>
       <c r="T45" s="16"/>
       <c r="U45" s="9"/>
     </row>
@@ -3781,25 +3745,24 @@
       <c r="E46" s="25">
         <v>256</v>
       </c>
-      <c r="F46" s="49">
+      <c r="F46" s="34">
         <v>320</v>
       </c>
       <c r="G46" s="2">
         <v>1733</v>
       </c>
-      <c r="H46" s="58">
+      <c r="H46" s="43">
         <v>8</v>
       </c>
-      <c r="I46" s="29" t="str">
-        <f>ВПР(A46;M:N;2;0)</f>
-        <v>30-37Mh/s</v>
+      <c r="I46" s="29" t="s">
+        <v>38</v>
       </c>
       <c r="J46"/>
-      <c r="K46" s="55">
+      <c r="K46" s="40">
         <f t="shared" si="0"/>
-        <v>37.687334768093578</v>
-      </c>
-      <c r="M46" s="32"/>
+        <v>37.236363636363642</v>
+      </c>
+      <c r="M46" s="47"/>
       <c r="N46" s="17" t="s">
         <v>72</v>
       </c>
@@ -3807,7 +3770,7 @@
       <c r="P46" s="17"/>
       <c r="Q46" s="17"/>
       <c r="R46" s="17"/>
-      <c r="S46" s="34"/>
+      <c r="S46" s="49"/>
       <c r="T46" s="17"/>
       <c r="U46" s="10"/>
     </row>
@@ -3833,30 +3796,29 @@
       <c r="G47" s="2">
         <v>1582</v>
       </c>
-      <c r="H47" s="58">
+      <c r="H47" s="43">
         <v>11</v>
       </c>
-      <c r="I47" s="29" t="str">
-        <f>ВПР(A47;M:N;2;0)</f>
-        <v> 40-50Mh/s</v>
+      <c r="I47" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="J47"/>
-      <c r="K47" s="55">
+      <c r="K47" s="40">
         <f t="shared" si="0"/>
-        <v>74.423222764578995</v>
-      </c>
-      <c r="M47" s="31" t="s">
+        <v>74.504356919578868</v>
+      </c>
+      <c r="M47" s="46" t="s">
         <v>73</v>
       </c>
       <c r="N47" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="O47" s="33"/>
-      <c r="P47" s="33"/>
-      <c r="Q47" s="33"/>
-      <c r="R47" s="33"/>
-      <c r="S47" s="33"/>
-      <c r="T47" s="35"/>
+      <c r="O47" s="48"/>
+      <c r="P47" s="48"/>
+      <c r="Q47" s="48"/>
+      <c r="R47" s="48"/>
+      <c r="S47" s="48"/>
+      <c r="T47" s="50"/>
       <c r="U47" s="9"/>
     </row>
     <row r="48" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3881,26 +3843,25 @@
       <c r="G48" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H48" s="56"/>
+      <c r="H48" s="41"/>
       <c r="I48" s="29" t="e">
-        <f>ВПР(A48;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J48"/>
-      <c r="K48" s="55" t="e">
-        <f t="shared" ref="K6:K69" si="1">КОРЕНЬ(B48) *  КОРЕНЬ(E48) * (КОРЕНЬ(F48) + 1)  * КОРЕНЬ(H48)/ 4720,7 * 4,2</f>
+      <c r="K48" s="40" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M48" s="32"/>
+      <c r="M48" s="47"/>
       <c r="N48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="O48" s="34"/>
-      <c r="P48" s="34"/>
-      <c r="Q48" s="34"/>
-      <c r="R48" s="34"/>
-      <c r="S48" s="34"/>
-      <c r="T48" s="36"/>
+      <c r="O48" s="49"/>
+      <c r="P48" s="49"/>
+      <c r="Q48" s="49"/>
+      <c r="R48" s="49"/>
+      <c r="S48" s="49"/>
+      <c r="T48" s="51"/>
       <c r="U48" s="10"/>
     </row>
     <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3921,29 +3882,28 @@
       <c r="G49" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H49" s="57" t="s">
+      <c r="H49" s="42" t="s">
         <v>230</v>
       </c>
       <c r="I49" s="29" t="e">
-        <f>ВПР(A49;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J49"/>
-      <c r="K49" s="55" t="e">
-        <f t="shared" si="1"/>
+      <c r="K49" s="40" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M49" s="31" t="s">
+      <c r="M49" s="46" t="s">
         <v>74</v>
       </c>
       <c r="N49" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="O49" s="33"/>
-      <c r="P49" s="33"/>
-      <c r="Q49" s="33"/>
+      <c r="O49" s="48"/>
+      <c r="P49" s="48"/>
+      <c r="Q49" s="48"/>
       <c r="R49" s="16"/>
-      <c r="S49" s="33"/>
+      <c r="S49" s="48"/>
       <c r="T49" s="16"/>
       <c r="U49" s="9"/>
     </row>
@@ -3961,25 +3921,24 @@
         <v>9</v>
       </c>
       <c r="G50" s="4"/>
-      <c r="H50" s="56"/>
+      <c r="H50" s="41"/>
       <c r="I50" s="29" t="e">
-        <f>ВПР(A50;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J50"/>
-      <c r="K50" s="55" t="e">
-        <f t="shared" si="1"/>
+      <c r="K50" s="40" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M50" s="32"/>
+      <c r="M50" s="47"/>
       <c r="N50" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="O50" s="34"/>
-      <c r="P50" s="34"/>
-      <c r="Q50" s="34"/>
+      <c r="O50" s="49"/>
+      <c r="P50" s="49"/>
+      <c r="Q50" s="49"/>
       <c r="R50" s="17"/>
-      <c r="S50" s="34"/>
+      <c r="S50" s="49"/>
       <c r="T50" s="17"/>
       <c r="U50" s="10"/>
     </row>
@@ -4005,27 +3964,26 @@
       <c r="G51" s="5">
         <v>1188</v>
       </c>
-      <c r="H51" s="58"/>
+      <c r="H51" s="43"/>
       <c r="I51" s="29" t="e">
-        <f>ВПР(A51;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J51"/>
-      <c r="K51" s="55">
-        <f t="shared" si="1"/>
+      <c r="K51" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M51" s="31" t="s">
+      <c r="M51" s="46" t="s">
         <v>75</v>
       </c>
       <c r="N51" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="O51" s="33"/>
-      <c r="P51" s="33"/>
+      <c r="O51" s="48"/>
+      <c r="P51" s="48"/>
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
-      <c r="S51" s="33"/>
+      <c r="S51" s="48"/>
       <c r="T51" s="16"/>
       <c r="U51" s="9"/>
     </row>
@@ -4051,25 +4009,24 @@
       <c r="G52" s="5">
         <v>1178</v>
       </c>
-      <c r="H52" s="58"/>
+      <c r="H52" s="43"/>
       <c r="I52" s="29" t="e">
-        <f>ВПР(A52;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J52"/>
-      <c r="K52" s="55">
-        <f t="shared" si="1"/>
+      <c r="K52" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M52" s="32"/>
+      <c r="M52" s="47"/>
       <c r="N52" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="O52" s="34"/>
-      <c r="P52" s="34"/>
+      <c r="O52" s="49"/>
+      <c r="P52" s="49"/>
       <c r="Q52" s="17"/>
       <c r="R52" s="17"/>
-      <c r="S52" s="34"/>
+      <c r="S52" s="49"/>
       <c r="T52" s="17"/>
       <c r="U52" s="10"/>
     </row>
@@ -4095,28 +4052,27 @@
       <c r="G53" s="5">
         <v>1178</v>
       </c>
-      <c r="H53" s="58"/>
+      <c r="H53" s="43"/>
       <c r="I53" s="29" t="e">
-        <f>ВПР(A53;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J53"/>
-      <c r="K53" s="55">
-        <f t="shared" si="1"/>
+      <c r="K53" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M53" s="31" t="s">
+      <c r="M53" s="46" t="s">
         <v>78</v>
       </c>
       <c r="N53" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="O53" s="33"/>
-      <c r="P53" s="33"/>
-      <c r="Q53" s="33"/>
-      <c r="R53" s="33"/>
-      <c r="S53" s="33"/>
-      <c r="T53" s="35"/>
+      <c r="O53" s="48"/>
+      <c r="P53" s="48"/>
+      <c r="Q53" s="48"/>
+      <c r="R53" s="48"/>
+      <c r="S53" s="48"/>
+      <c r="T53" s="50"/>
       <c r="U53" s="9"/>
     </row>
     <row r="54" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4141,26 +4097,25 @@
       <c r="G54" s="5">
         <v>1216</v>
       </c>
-      <c r="H54" s="58"/>
+      <c r="H54" s="43"/>
       <c r="I54" s="29" t="e">
-        <f>ВПР(A54;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J54"/>
-      <c r="K54" s="55">
-        <f t="shared" si="1"/>
+      <c r="K54" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M54" s="32"/>
+      <c r="M54" s="47"/>
       <c r="N54" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="O54" s="34"/>
-      <c r="P54" s="34"/>
-      <c r="Q54" s="34"/>
-      <c r="R54" s="34"/>
-      <c r="S54" s="34"/>
-      <c r="T54" s="36"/>
+      <c r="O54" s="49"/>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
+      <c r="R54" s="49"/>
+      <c r="S54" s="49"/>
+      <c r="T54" s="51"/>
       <c r="U54" s="10"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -4185,27 +4140,26 @@
       <c r="G55" s="5">
         <v>1075</v>
       </c>
-      <c r="H55" s="58"/>
+      <c r="H55" s="43"/>
       <c r="I55" s="29" t="e">
-        <f>ВПР(A55;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J55"/>
-      <c r="K55" s="55">
-        <f t="shared" si="1"/>
+      <c r="K55" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M55" s="31" t="s">
+      <c r="M55" s="46" t="s">
         <v>79</v>
       </c>
       <c r="N55" s="16" t="s">
         <v>224</v>
       </c>
       <c r="O55" s="16"/>
-      <c r="P55" s="33"/>
+      <c r="P55" s="48"/>
       <c r="Q55" s="16"/>
       <c r="R55" s="16"/>
-      <c r="S55" s="33"/>
+      <c r="S55" s="48"/>
       <c r="T55" s="16"/>
       <c r="U55" s="9"/>
     </row>
@@ -4217,25 +4171,24 @@
       <c r="E56" s="27"/>
       <c r="F56" s="27"/>
       <c r="G56" s="5"/>
-      <c r="H56" s="58"/>
+      <c r="H56" s="43"/>
       <c r="I56" s="29" t="e">
-        <f>ВПР(A56;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J56"/>
-      <c r="K56" s="55">
-        <f t="shared" si="1"/>
+      <c r="K56" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M56" s="32"/>
+      <c r="M56" s="47"/>
       <c r="N56" s="17" t="s">
         <v>62</v>
       </c>
       <c r="O56" s="17"/>
-      <c r="P56" s="34"/>
+      <c r="P56" s="49"/>
       <c r="Q56" s="17"/>
       <c r="R56" s="17"/>
-      <c r="S56" s="34"/>
+      <c r="S56" s="49"/>
       <c r="T56" s="17"/>
       <c r="U56" s="10"/>
     </row>
@@ -4261,23 +4214,22 @@
       <c r="G57" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H57" s="56"/>
+      <c r="H57" s="41"/>
       <c r="I57" s="29" t="e">
-        <f>ВПР(A57;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J57"/>
-      <c r="K57" s="55" t="e">
-        <f t="shared" si="1"/>
+      <c r="K57" s="40" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M57" s="31" t="s">
+      <c r="M57" s="46" t="s">
         <v>81</v>
       </c>
       <c r="N57" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="O57" s="33"/>
+      <c r="O57" s="48"/>
       <c r="P57" s="16"/>
       <c r="Q57" s="16"/>
       <c r="R57" s="16"/>
@@ -4303,23 +4255,22 @@
       <c r="G58" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H58" s="57" t="s">
+      <c r="H58" s="42" t="s">
         <v>230</v>
       </c>
       <c r="I58" s="29" t="e">
-        <f>ВПР(A58;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J58"/>
-      <c r="K58" s="55" t="e">
-        <f t="shared" si="1"/>
+      <c r="K58" s="40" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M58" s="32"/>
+      <c r="M58" s="47"/>
       <c r="N58" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="O58" s="34"/>
+      <c r="O58" s="49"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="17"/>
       <c r="R58" s="17"/>
@@ -4341,29 +4292,28 @@
         <v>9</v>
       </c>
       <c r="G59" s="4"/>
-      <c r="H59" s="56"/>
+      <c r="H59" s="41"/>
       <c r="I59" s="29" t="e">
-        <f>ВПР(A59;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J59"/>
-      <c r="K59" s="55" t="e">
-        <f t="shared" si="1"/>
+      <c r="K59" s="40" t="e">
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M59" s="31" t="s">
+      <c r="M59" s="46" t="s">
         <v>83</v>
       </c>
       <c r="N59" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="O59" s="33"/>
-      <c r="P59" s="33"/>
-      <c r="Q59" s="33"/>
-      <c r="R59" s="33"/>
-      <c r="S59" s="33"/>
+      <c r="O59" s="48"/>
+      <c r="P59" s="48"/>
+      <c r="Q59" s="48"/>
+      <c r="R59" s="48"/>
+      <c r="S59" s="48"/>
       <c r="T59" s="16"/>
-      <c r="U59" s="37"/>
+      <c r="U59" s="52"/>
     </row>
     <row r="60" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
@@ -4385,27 +4335,26 @@
         <v>44665</v>
       </c>
       <c r="G60" s="5"/>
-      <c r="H60" s="58"/>
+      <c r="H60" s="43"/>
       <c r="I60" s="29" t="e">
-        <f>ВПР(A60;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J60"/>
-      <c r="K60" s="55">
-        <f t="shared" si="1"/>
+      <c r="K60" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M60" s="32"/>
+      <c r="M60" s="47"/>
       <c r="N60" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="O60" s="34"/>
-      <c r="P60" s="34"/>
-      <c r="Q60" s="34"/>
-      <c r="R60" s="34"/>
-      <c r="S60" s="34"/>
+      <c r="O60" s="49"/>
+      <c r="P60" s="49"/>
+      <c r="Q60" s="49"/>
+      <c r="R60" s="49"/>
+      <c r="S60" s="49"/>
       <c r="T60" s="17"/>
-      <c r="U60" s="38"/>
+      <c r="U60" s="53"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
@@ -4427,27 +4376,26 @@
         <v>40</v>
       </c>
       <c r="G61" s="5"/>
-      <c r="H61" s="58"/>
+      <c r="H61" s="43"/>
       <c r="I61" s="29" t="e">
-        <f>ВПР(A61;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J61"/>
-      <c r="K61" s="55">
-        <f t="shared" si="1"/>
+      <c r="K61" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M61" s="31" t="s">
+      <c r="M61" s="46" t="s">
         <v>85</v>
       </c>
       <c r="N61" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="O61" s="33"/>
-      <c r="P61" s="33"/>
-      <c r="Q61" s="33"/>
+      <c r="O61" s="48"/>
+      <c r="P61" s="48"/>
+      <c r="Q61" s="48"/>
       <c r="R61" s="16"/>
-      <c r="S61" s="33"/>
+      <c r="S61" s="48"/>
       <c r="T61" s="16"/>
       <c r="U61" s="9"/>
     </row>
@@ -4471,25 +4419,24 @@
         <v>44801</v>
       </c>
       <c r="G62" s="5"/>
-      <c r="H62" s="58"/>
+      <c r="H62" s="43"/>
       <c r="I62" s="29" t="e">
-        <f>ВПР(A62;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J62"/>
-      <c r="K62" s="55">
-        <f t="shared" si="1"/>
+      <c r="K62" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M62" s="32"/>
+      <c r="M62" s="47"/>
       <c r="N62" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="O62" s="34"/>
-      <c r="P62" s="34"/>
-      <c r="Q62" s="34"/>
+      <c r="O62" s="49"/>
+      <c r="P62" s="49"/>
+      <c r="Q62" s="49"/>
       <c r="R62" s="17"/>
-      <c r="S62" s="34"/>
+      <c r="S62" s="49"/>
       <c r="T62" s="17"/>
       <c r="U62" s="10"/>
     </row>
@@ -4513,17 +4460,16 @@
         <v>44665</v>
       </c>
       <c r="G63" s="5"/>
-      <c r="H63" s="58"/>
+      <c r="H63" s="43"/>
       <c r="I63" s="29" t="e">
-        <f>ВПР(A63;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J63"/>
-      <c r="K63" s="55">
-        <f t="shared" si="1"/>
+      <c r="K63" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M63" s="31" t="s">
+      <c r="M63" s="46" t="s">
         <v>87</v>
       </c>
       <c r="N63" s="16" t="s">
@@ -4531,9 +4477,9 @@
       </c>
       <c r="O63" s="16"/>
       <c r="P63" s="16"/>
-      <c r="Q63" s="33"/>
+      <c r="Q63" s="48"/>
       <c r="R63" s="16"/>
-      <c r="S63" s="33"/>
+      <c r="S63" s="48"/>
       <c r="T63" s="16"/>
       <c r="U63" s="9"/>
     </row>
@@ -4557,25 +4503,24 @@
         <v>40</v>
       </c>
       <c r="G64" s="5"/>
-      <c r="H64" s="58"/>
+      <c r="H64" s="43"/>
       <c r="I64" s="29" t="e">
-        <f>ВПР(A64;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J64"/>
-      <c r="K64" s="55">
-        <f t="shared" si="1"/>
+      <c r="K64" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M64" s="32"/>
+      <c r="M64" s="47"/>
       <c r="N64" s="17" t="s">
         <v>41</v>
       </c>
       <c r="O64" s="17"/>
       <c r="P64" s="17"/>
-      <c r="Q64" s="34"/>
+      <c r="Q64" s="49"/>
       <c r="R64" s="17"/>
-      <c r="S64" s="34"/>
+      <c r="S64" s="49"/>
       <c r="T64" s="17"/>
       <c r="U64" s="10"/>
     </row>
@@ -4599,28 +4544,27 @@
         <v>44801</v>
       </c>
       <c r="G65" s="5"/>
-      <c r="H65" s="58"/>
+      <c r="H65" s="43"/>
       <c r="I65" s="29" t="e">
-        <f>ВПР(A65;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J65"/>
-      <c r="K65" s="55">
-        <f t="shared" si="1"/>
+      <c r="K65" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M65" s="31" t="s">
+      <c r="M65" s="46" t="s">
         <v>89</v>
       </c>
       <c r="N65" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="O65" s="33"/>
-      <c r="P65" s="33"/>
-      <c r="Q65" s="33"/>
-      <c r="R65" s="33"/>
-      <c r="S65" s="33"/>
-      <c r="T65" s="35"/>
+      <c r="O65" s="48"/>
+      <c r="P65" s="48"/>
+      <c r="Q65" s="48"/>
+      <c r="R65" s="48"/>
+      <c r="S65" s="48"/>
+      <c r="T65" s="50"/>
       <c r="U65" s="9"/>
     </row>
     <row r="66" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4643,26 +4587,25 @@
         <v>80</v>
       </c>
       <c r="G66" s="5"/>
-      <c r="H66" s="58"/>
+      <c r="H66" s="43"/>
       <c r="I66" s="29" t="e">
-        <f>ВПР(A66;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J66"/>
-      <c r="K66" s="55">
-        <f t="shared" si="1"/>
+      <c r="K66" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M66" s="32"/>
+      <c r="M66" s="47"/>
       <c r="N66" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="O66" s="34"/>
-      <c r="P66" s="34"/>
-      <c r="Q66" s="34"/>
-      <c r="R66" s="34"/>
-      <c r="S66" s="34"/>
-      <c r="T66" s="36"/>
+      <c r="O66" s="49"/>
+      <c r="P66" s="49"/>
+      <c r="Q66" s="49"/>
+      <c r="R66" s="49"/>
+      <c r="S66" s="49"/>
+      <c r="T66" s="51"/>
       <c r="U66" s="10"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
@@ -4685,25 +4628,24 @@
         <v>44801</v>
       </c>
       <c r="G67" s="5"/>
-      <c r="H67" s="58"/>
+      <c r="H67" s="43"/>
       <c r="I67" s="29" t="e">
-        <f>ВПР(A67;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J67"/>
-      <c r="K67" s="55">
-        <f t="shared" si="1"/>
+      <c r="K67" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M67" s="31" t="s">
+      <c r="M67" s="46" t="s">
         <v>92</v>
       </c>
       <c r="N67" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="O67" s="33"/>
-      <c r="P67" s="33"/>
-      <c r="Q67" s="33"/>
+      <c r="O67" s="48"/>
+      <c r="P67" s="48"/>
+      <c r="Q67" s="48"/>
       <c r="R67" s="16"/>
       <c r="S67" s="16"/>
       <c r="T67" s="16"/>
@@ -4731,23 +4673,22 @@
       <c r="G68" s="5">
         <v>1085</v>
       </c>
-      <c r="H68" s="58"/>
+      <c r="H68" s="43"/>
       <c r="I68" s="29" t="e">
-        <f>ВПР(A68;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J68"/>
-      <c r="K68" s="55">
-        <f t="shared" si="1"/>
+      <c r="K68" s="40">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M68" s="32"/>
+      <c r="M68" s="47"/>
       <c r="N68" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O68" s="34"/>
-      <c r="P68" s="34"/>
-      <c r="Q68" s="34"/>
+      <c r="O68" s="49"/>
+      <c r="P68" s="49"/>
+      <c r="Q68" s="49"/>
       <c r="R68" s="17"/>
       <c r="S68" s="17"/>
       <c r="T68" s="17"/>
@@ -4775,27 +4716,26 @@
       <c r="G69" s="5">
         <v>1085</v>
       </c>
-      <c r="H69" s="58"/>
+      <c r="H69" s="43"/>
       <c r="I69" s="29" t="e">
-        <f>ВПР(A69;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J69"/>
-      <c r="K69" s="55" t="e">
-        <f t="shared" si="1"/>
+      <c r="K69" s="40" t="e">
+        <f t="shared" ref="K69:K121" si="1" xml:space="preserve"> SQRT(B69) * SQRT(E69) * IF(F69 &gt; 600, LOG(F69), SQRT(F69)) * IF(F69&lt;190, 1.1, 1) * ( SQRT(H69) * IF(H69 &lt; 5, 1.1, 1) ) / IF(F69 &gt; 600, 140, 1100) * IF(B69&lt;1300,  IF(B69&gt;1000, 1.4, 2 ), 1 )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M69" s="31" t="s">
+      <c r="M69" s="46" t="s">
         <v>94</v>
       </c>
       <c r="N69" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="O69" s="33"/>
-      <c r="P69" s="33"/>
-      <c r="Q69" s="33"/>
-      <c r="R69" s="33"/>
-      <c r="S69" s="33"/>
+      <c r="O69" s="48"/>
+      <c r="P69" s="48"/>
+      <c r="Q69" s="48"/>
+      <c r="R69" s="48"/>
+      <c r="S69" s="48"/>
       <c r="T69" s="16"/>
       <c r="U69" s="9"/>
     </row>
@@ -4821,25 +4761,24 @@
       <c r="G70" s="5">
         <v>1033</v>
       </c>
-      <c r="H70" s="58"/>
+      <c r="H70" s="43"/>
       <c r="I70" s="29" t="e">
-        <f>ВПР(A70;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J70"/>
-      <c r="K70" s="55" t="e">
-        <f t="shared" ref="K70:K100" si="2">КОРЕНЬ(B70) *  КОРЕНЬ(E70) * (КОРЕНЬ(F70) + 1)  * КОРЕНЬ(H70)/ 4720,7 * 4,2</f>
+      <c r="K70" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M70" s="32"/>
+      <c r="M70" s="47"/>
       <c r="N70" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="O70" s="34"/>
-      <c r="P70" s="34"/>
-      <c r="Q70" s="34"/>
-      <c r="R70" s="34"/>
-      <c r="S70" s="34"/>
+      <c r="O70" s="49"/>
+      <c r="P70" s="49"/>
+      <c r="Q70" s="49"/>
+      <c r="R70" s="49"/>
+      <c r="S70" s="49"/>
       <c r="T70" s="17"/>
       <c r="U70" s="10"/>
     </row>
@@ -4865,17 +4804,16 @@
       <c r="G71" s="3">
         <v>888</v>
       </c>
-      <c r="H71" s="58"/>
+      <c r="H71" s="43"/>
       <c r="I71" s="29" t="e">
-        <f>ВПР(A71;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J71"/>
-      <c r="K71" s="55">
-        <f t="shared" si="2"/>
+      <c r="K71" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M71" s="31" t="s">
+      <c r="M71" s="46" t="s">
         <v>96</v>
       </c>
       <c r="N71" s="16" t="s">
@@ -4883,9 +4821,9 @@
       </c>
       <c r="O71" s="16"/>
       <c r="P71" s="16"/>
-      <c r="Q71" s="33"/>
-      <c r="R71" s="33"/>
-      <c r="S71" s="33"/>
+      <c r="Q71" s="48"/>
+      <c r="R71" s="48"/>
+      <c r="S71" s="48"/>
       <c r="T71" s="16"/>
       <c r="U71" s="9"/>
     </row>
@@ -4911,25 +4849,24 @@
       <c r="G72" s="3">
         <v>1033</v>
       </c>
-      <c r="H72" s="58"/>
+      <c r="H72" s="43"/>
       <c r="I72" s="29" t="e">
-        <f>ВПР(A72;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J72"/>
-      <c r="K72" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K72" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M72" s="32"/>
+      <c r="M72" s="47"/>
       <c r="N72" s="17" t="s">
         <v>40</v>
       </c>
       <c r="O72" s="17"/>
       <c r="P72" s="17"/>
-      <c r="Q72" s="34"/>
-      <c r="R72" s="34"/>
-      <c r="S72" s="34"/>
+      <c r="Q72" s="49"/>
+      <c r="R72" s="49"/>
+      <c r="S72" s="49"/>
       <c r="T72" s="17"/>
       <c r="U72" s="10"/>
     </row>
@@ -4955,17 +4892,16 @@
       <c r="G73" s="5">
         <v>1085</v>
       </c>
-      <c r="H73" s="58"/>
+      <c r="H73" s="43"/>
       <c r="I73" s="29" t="e">
-        <f>ВПР(A73;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J73"/>
-      <c r="K73" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K73" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M73" s="39" t="s">
+      <c r="M73" s="54" t="s">
         <v>98</v>
       </c>
       <c r="N73" s="18" t="s">
@@ -4973,8 +4909,8 @@
       </c>
       <c r="O73" s="18"/>
       <c r="P73" s="18"/>
-      <c r="Q73" s="41"/>
-      <c r="R73" s="41"/>
+      <c r="Q73" s="56"/>
+      <c r="R73" s="56"/>
       <c r="T73" s="20"/>
       <c r="U73" s="9"/>
     </row>
@@ -5000,24 +4936,23 @@
       <c r="G74" s="5">
         <v>900</v>
       </c>
-      <c r="H74" s="58"/>
+      <c r="H74" s="43"/>
       <c r="I74" s="29" t="e">
-        <f>ВПР(A74;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J74"/>
-      <c r="K74" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K74" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M74" s="40"/>
+      <c r="M74" s="55"/>
       <c r="N74" s="19" t="s">
         <v>100</v>
       </c>
       <c r="O74" s="19"/>
       <c r="P74" s="19"/>
-      <c r="Q74" s="42"/>
-      <c r="R74" s="42"/>
+      <c r="Q74" s="57"/>
+      <c r="R74" s="57"/>
       <c r="S74" s="21"/>
       <c r="T74" s="22"/>
       <c r="U74" s="10"/>
@@ -5044,23 +4979,22 @@
       <c r="G75" s="5">
         <v>928</v>
       </c>
-      <c r="H75" s="58"/>
+      <c r="H75" s="43"/>
       <c r="I75" s="29" t="e">
-        <f>ВПР(A75;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J75"/>
-      <c r="K75" s="55">
-        <f t="shared" si="2"/>
+      <c r="K75" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M75" s="37"/>
+      <c r="M75" s="52"/>
       <c r="N75" s="6"/>
-      <c r="O75" s="37"/>
-      <c r="P75" s="37"/>
-      <c r="Q75" s="37"/>
+      <c r="O75" s="52"/>
+      <c r="P75" s="52"/>
+      <c r="Q75" s="52"/>
       <c r="R75" s="6"/>
-      <c r="S75" s="37"/>
+      <c r="S75" s="52"/>
       <c r="T75" s="6"/>
       <c r="U75" s="9"/>
     </row>
@@ -5072,23 +5006,22 @@
       <c r="E76" s="27"/>
       <c r="F76" s="27"/>
       <c r="G76" s="5"/>
-      <c r="H76" s="58"/>
+      <c r="H76" s="43"/>
       <c r="I76" s="29" t="e">
-        <f>ВПР(A76;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J76"/>
-      <c r="K76" s="55">
-        <f t="shared" si="2"/>
+      <c r="K76" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M76" s="38"/>
+      <c r="M76" s="53"/>
       <c r="N76" s="7"/>
-      <c r="O76" s="38"/>
-      <c r="P76" s="38"/>
-      <c r="Q76" s="38"/>
+      <c r="O76" s="53"/>
+      <c r="P76" s="53"/>
+      <c r="Q76" s="53"/>
       <c r="R76" s="7"/>
-      <c r="S76" s="38"/>
+      <c r="S76" s="53"/>
       <c r="T76" s="7"/>
       <c r="U76" s="10"/>
     </row>
@@ -5114,24 +5047,23 @@
       <c r="G77" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H77" s="56"/>
+      <c r="H77" s="41"/>
       <c r="I77" s="29" t="e">
-        <f>ВПР(A77;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J77"/>
-      <c r="K77" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K77" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M77" s="37"/>
+      <c r="M77" s="52"/>
       <c r="N77" s="6"/>
-      <c r="O77" s="37"/>
-      <c r="P77" s="37"/>
-      <c r="Q77" s="37"/>
-      <c r="R77" s="37"/>
-      <c r="S77" s="37"/>
-      <c r="T77" s="37"/>
+      <c r="O77" s="52"/>
+      <c r="P77" s="52"/>
+      <c r="Q77" s="52"/>
+      <c r="R77" s="52"/>
+      <c r="S77" s="52"/>
+      <c r="T77" s="52"/>
       <c r="U77" s="9"/>
     </row>
     <row r="78" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5152,26 +5084,25 @@
       <c r="G78" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H78" s="57" t="s">
+      <c r="H78" s="42" t="s">
         <v>230</v>
       </c>
       <c r="I78" s="29" t="e">
-        <f>ВПР(A78;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J78"/>
-      <c r="K78" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K78" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M78" s="38"/>
+      <c r="M78" s="53"/>
       <c r="N78" s="7"/>
-      <c r="O78" s="38"/>
-      <c r="P78" s="38"/>
-      <c r="Q78" s="38"/>
-      <c r="R78" s="38"/>
-      <c r="S78" s="38"/>
-      <c r="T78" s="38"/>
+      <c r="O78" s="53"/>
+      <c r="P78" s="53"/>
+      <c r="Q78" s="53"/>
+      <c r="R78" s="53"/>
+      <c r="S78" s="53"/>
+      <c r="T78" s="53"/>
       <c r="U78" s="10"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
@@ -5188,24 +5119,23 @@
         <v>9</v>
       </c>
       <c r="G79" s="4"/>
-      <c r="H79" s="56"/>
+      <c r="H79" s="41"/>
       <c r="I79" s="29" t="e">
-        <f>ВПР(A79;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J79"/>
-      <c r="K79" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K79" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M79" s="37"/>
+      <c r="M79" s="52"/>
       <c r="N79" s="6"/>
       <c r="O79" s="6"/>
       <c r="P79" s="6"/>
-      <c r="Q79" s="37"/>
-      <c r="R79" s="37"/>
-      <c r="S79" s="37"/>
-      <c r="T79" s="37"/>
+      <c r="Q79" s="52"/>
+      <c r="R79" s="52"/>
+      <c r="S79" s="52"/>
+      <c r="T79" s="52"/>
       <c r="U79" s="9"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5230,24 +5160,23 @@
       <c r="G80" s="3">
         <v>1046</v>
       </c>
-      <c r="H80" s="58"/>
+      <c r="H80" s="43"/>
       <c r="I80" s="29" t="e">
-        <f>ВПР(A80;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J80"/>
-      <c r="K80" s="55">
-        <f t="shared" si="2"/>
+      <c r="K80" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M80" s="38"/>
+      <c r="M80" s="53"/>
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
       <c r="P80" s="7"/>
-      <c r="Q80" s="38"/>
-      <c r="R80" s="38"/>
-      <c r="S80" s="38"/>
-      <c r="T80" s="38"/>
+      <c r="Q80" s="53"/>
+      <c r="R80" s="53"/>
+      <c r="S80" s="53"/>
+      <c r="T80" s="53"/>
       <c r="U80" s="10"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
@@ -5272,24 +5201,23 @@
       <c r="G81" s="5">
         <v>900</v>
       </c>
-      <c r="H81" s="58"/>
+      <c r="H81" s="43"/>
       <c r="I81" s="29" t="e">
-        <f>ВПР(A81;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J81"/>
-      <c r="K81" s="55">
-        <f t="shared" si="2"/>
+      <c r="K81" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M81" s="43"/>
+      <c r="M81" s="58"/>
       <c r="N81" s="8"/>
       <c r="O81" s="8"/>
       <c r="P81" s="8"/>
-      <c r="Q81" s="43"/>
-      <c r="R81" s="43"/>
-      <c r="S81" s="43"/>
-      <c r="T81" s="43"/>
+      <c r="Q81" s="58"/>
+      <c r="R81" s="58"/>
+      <c r="S81" s="58"/>
+      <c r="T81" s="58"/>
       <c r="U81" s="12"/>
     </row>
     <row r="82" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5314,24 +5242,23 @@
       <c r="G82" s="3">
         <v>1620</v>
       </c>
-      <c r="H82" s="58"/>
+      <c r="H82" s="43"/>
       <c r="I82" s="29" t="e">
-        <f>ВПР(A82;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J82"/>
-      <c r="K82" s="55">
-        <f t="shared" si="2"/>
+      <c r="K82" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M82" s="44"/>
+      <c r="M82" s="59"/>
       <c r="N82" s="13"/>
       <c r="O82" s="13"/>
       <c r="P82" s="13"/>
-      <c r="Q82" s="44"/>
-      <c r="R82" s="44"/>
-      <c r="S82" s="44"/>
-      <c r="T82" s="44"/>
+      <c r="Q82" s="59"/>
+      <c r="R82" s="59"/>
+      <c r="S82" s="59"/>
+      <c r="T82" s="59"/>
       <c r="U82" s="14"/>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
@@ -5356,14 +5283,13 @@
       <c r="G83" s="5">
         <v>1400</v>
       </c>
-      <c r="H83" s="58"/>
+      <c r="H83" s="43"/>
       <c r="I83" s="29" t="e">
-        <f>ВПР(A83;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J83"/>
-      <c r="K83" s="55">
-        <f t="shared" si="2"/>
+      <c r="K83" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5389,14 +5315,13 @@
       <c r="G84" s="3">
         <v>875</v>
       </c>
-      <c r="H84" s="58"/>
+      <c r="H84" s="43"/>
       <c r="I84" s="29" t="e">
-        <f>ВПР(A84;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J84"/>
-      <c r="K84" s="55">
-        <f t="shared" si="2"/>
+      <c r="K84" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5422,14 +5347,13 @@
       <c r="G85" s="5">
         <v>1620</v>
       </c>
-      <c r="H85" s="58"/>
+      <c r="H85" s="43"/>
       <c r="I85" s="29" t="e">
-        <f>ВПР(A85;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J85"/>
-      <c r="K85" s="55">
-        <f t="shared" si="2"/>
+      <c r="K85" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5455,14 +5379,13 @@
       <c r="G86" s="5">
         <v>1620</v>
       </c>
-      <c r="H86" s="58"/>
+      <c r="H86" s="43"/>
       <c r="I86" s="29" t="e">
-        <f>ВПР(A86;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J86"/>
-      <c r="K86" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K86" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5488,14 +5411,13 @@
       <c r="G87" s="5">
         <v>900</v>
       </c>
-      <c r="H87" s="58"/>
+      <c r="H87" s="43"/>
       <c r="I87" s="29" t="e">
-        <f>ВПР(A87;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J87"/>
-      <c r="K87" s="55">
-        <f t="shared" si="2"/>
+      <c r="K87" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5521,14 +5443,13 @@
       <c r="G88" s="3">
         <v>797</v>
       </c>
-      <c r="H88" s="58"/>
+      <c r="H88" s="43"/>
       <c r="I88" s="29" t="e">
-        <f>ВПР(A88;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J88"/>
-      <c r="K88" s="55">
-        <f t="shared" si="2"/>
+      <c r="K88" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5554,14 +5475,13 @@
       <c r="G89" s="3">
         <v>1440</v>
       </c>
-      <c r="H89" s="58"/>
+      <c r="H89" s="43"/>
       <c r="I89" s="29" t="e">
-        <f>ВПР(A89;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J89"/>
-      <c r="K89" s="55">
-        <f t="shared" si="2"/>
+      <c r="K89" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5587,14 +5507,13 @@
       <c r="G90" s="3">
         <v>950</v>
       </c>
-      <c r="H90" s="58"/>
+      <c r="H90" s="43"/>
       <c r="I90" s="29" t="e">
-        <f>ВПР(A90;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J90"/>
-      <c r="K90" s="55">
-        <f t="shared" si="2"/>
+      <c r="K90" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5620,14 +5539,13 @@
       <c r="G91" s="3">
         <v>1552</v>
       </c>
-      <c r="H91" s="58"/>
+      <c r="H91" s="43"/>
       <c r="I91" s="29" t="e">
-        <f>ВПР(A91;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J91"/>
-      <c r="K91" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K91" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5653,14 +5571,13 @@
       <c r="G92" s="5">
         <v>1058</v>
       </c>
-      <c r="H92" s="58"/>
+      <c r="H92" s="43"/>
       <c r="I92" s="29" t="e">
-        <f>ВПР(A92;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J92"/>
-      <c r="K92" s="55">
-        <f t="shared" si="2"/>
+      <c r="K92" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5686,14 +5603,13 @@
       <c r="G93" s="5">
         <v>928</v>
       </c>
-      <c r="H93" s="58"/>
+      <c r="H93" s="43"/>
       <c r="I93" s="29" t="e">
-        <f>ВПР(A93;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J93"/>
-      <c r="K93" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K93" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5719,14 +5635,13 @@
       <c r="G94" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H94" s="58"/>
+      <c r="H94" s="43"/>
       <c r="I94" s="29" t="e">
-        <f>ВПР(A94;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J94"/>
-      <c r="K94" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K94" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5738,14 +5653,13 @@
       <c r="E95" s="27"/>
       <c r="F95" s="27"/>
       <c r="G95" s="5"/>
-      <c r="H95" s="58"/>
+      <c r="H95" s="43"/>
       <c r="I95" s="29" t="e">
-        <f>ВПР(A95;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J95"/>
-      <c r="K95" s="55">
-        <f t="shared" si="2"/>
+      <c r="K95" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5771,14 +5685,13 @@
       <c r="G96" s="5">
         <v>980</v>
       </c>
-      <c r="H96" s="58"/>
+      <c r="H96" s="43"/>
       <c r="I96" s="29" t="e">
-        <f>ВПР(A96;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J96"/>
-      <c r="K96" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K96" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5804,14 +5717,13 @@
       <c r="G97" s="3">
         <v>823</v>
       </c>
-      <c r="H97" s="58"/>
+      <c r="H97" s="43"/>
       <c r="I97" s="29" t="e">
-        <f>ВПР(A97;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J97"/>
-      <c r="K97" s="55">
-        <f t="shared" si="2"/>
+      <c r="K97" s="40">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5837,14 +5749,13 @@
       <c r="G98" s="5">
         <v>980</v>
       </c>
-      <c r="H98" s="58"/>
+      <c r="H98" s="43"/>
       <c r="I98" s="29" t="e">
-        <f>ВПР(A98;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J98"/>
-      <c r="K98" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K98" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5870,14 +5781,13 @@
       <c r="G99" s="5">
         <v>980</v>
       </c>
-      <c r="H99" s="58"/>
+      <c r="H99" s="43"/>
       <c r="I99" s="29" t="e">
-        <f>ВПР(A99;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J99"/>
-      <c r="K99" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K99" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5903,14 +5813,13 @@
       <c r="G100" s="5">
         <v>1006</v>
       </c>
-      <c r="H100" s="58"/>
+      <c r="H100" s="43"/>
       <c r="I100" s="29" t="e">
-        <f>ВПР(A100;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J100"/>
-      <c r="K100" s="55" t="e">
-        <f t="shared" si="2"/>
+      <c r="K100" s="40" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5936,13 +5845,15 @@
       <c r="G101" s="5">
         <v>915</v>
       </c>
-      <c r="H101" s="58"/>
+      <c r="H101" s="43"/>
       <c r="I101" s="29" t="e">
-        <f>ВПР(A101;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J101"/>
-      <c r="K101" s="55"/>
+      <c r="K101" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="102" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
@@ -5966,13 +5877,15 @@
       <c r="G102" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H102" s="58"/>
+      <c r="H102" s="43"/>
       <c r="I102" s="29" t="e">
-        <f>ВПР(A102;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J102"/>
-      <c r="K102" s="55"/>
+      <c r="K102" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
@@ -5992,13 +5905,15 @@
       <c r="G103" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H103" s="58"/>
+      <c r="H103" s="43"/>
       <c r="I103" s="29" t="e">
-        <f>ВПР(A103;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J103"/>
-      <c r="K103" s="55"/>
+      <c r="K103" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
@@ -6014,13 +5929,15 @@
         <v>9</v>
       </c>
       <c r="G104" s="4"/>
-      <c r="H104" s="58"/>
+      <c r="H104" s="43"/>
       <c r="I104" s="29" t="e">
-        <f>ВПР(A104;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J104"/>
-      <c r="K104" s="55"/>
+      <c r="K104" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
@@ -6044,15 +5961,17 @@
       <c r="G105" s="3">
         <v>1620</v>
       </c>
-      <c r="H105" s="58"/>
+      <c r="H105" s="43"/>
       <c r="I105" s="29" t="e">
-        <f>ВПР(A105;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J105"/>
-      <c r="K105" s="55"/>
-    </row>
-    <row r="106" spans="1:11" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K105" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>176</v>
       </c>
@@ -6074,13 +5993,15 @@
       <c r="G106" s="5">
         <v>1024</v>
       </c>
-      <c r="H106" s="58"/>
+      <c r="H106" s="43"/>
       <c r="I106" s="29" t="e">
-        <f>ВПР(A106;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J106"/>
-      <c r="K106" s="55"/>
+      <c r="K106" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
@@ -6104,13 +6025,15 @@
       <c r="G107" s="3">
         <v>1400</v>
       </c>
-      <c r="H107" s="58"/>
+      <c r="H107" s="43"/>
       <c r="I107" s="29" t="e">
-        <f>ВПР(A107;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J107"/>
-      <c r="K107" s="55"/>
+      <c r="K107" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
@@ -6134,13 +6057,15 @@
       <c r="G108" s="5">
         <v>1440</v>
       </c>
-      <c r="H108" s="58"/>
+      <c r="H108" s="43"/>
       <c r="I108" s="29" t="e">
-        <f>ВПР(A108;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J108"/>
-      <c r="K108" s="55"/>
+      <c r="K108" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
@@ -6164,13 +6089,15 @@
       <c r="G109" s="3">
         <v>1740</v>
       </c>
-      <c r="H109" s="58"/>
+      <c r="H109" s="43"/>
       <c r="I109" s="29" t="e">
-        <f>ВПР(A109;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J109"/>
-      <c r="K109" s="55"/>
+      <c r="K109" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
@@ -6194,13 +6121,15 @@
       <c r="G110" s="5">
         <v>1800</v>
       </c>
-      <c r="H110" s="58"/>
+      <c r="H110" s="43"/>
       <c r="I110" s="29" t="e">
-        <f>ВПР(A110;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J110"/>
-      <c r="K110" s="55"/>
+      <c r="K110" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
@@ -6224,13 +6153,15 @@
       <c r="G111" s="3">
         <v>1553</v>
       </c>
-      <c r="H111" s="58"/>
+      <c r="H111" s="43"/>
       <c r="I111" s="29" t="e">
-        <f>ВПР(A111;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J111"/>
-      <c r="K111" s="55"/>
+      <c r="K111" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
@@ -6254,13 +6185,15 @@
       <c r="G112" s="3">
         <v>1104</v>
       </c>
-      <c r="H112" s="58"/>
+      <c r="H112" s="43"/>
       <c r="I112" s="29" t="e">
-        <f>ВПР(A112;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J112"/>
-      <c r="K112" s="55"/>
+      <c r="K112" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
@@ -6284,13 +6217,15 @@
       <c r="G113" s="5">
         <v>16201900</v>
       </c>
-      <c r="H113" s="58"/>
+      <c r="H113" s="43"/>
       <c r="I113" s="29" t="e">
-        <f>ВПР(A113;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J113"/>
-      <c r="K113" s="55"/>
+      <c r="K113" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
@@ -6314,13 +6249,15 @@
       <c r="G114" s="5">
         <v>1645</v>
       </c>
-      <c r="H114" s="58"/>
+      <c r="H114" s="43"/>
       <c r="I114" s="29" t="e">
-        <f>ВПР(A114;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J114"/>
-      <c r="K114" s="55"/>
+      <c r="K114" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
@@ -6344,13 +6281,15 @@
       <c r="G115" s="3">
         <v>1464</v>
       </c>
-      <c r="H115" s="58"/>
+      <c r="H115" s="43"/>
       <c r="I115" s="29" t="e">
-        <f>ВПР(A115;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J115"/>
-      <c r="K115" s="55"/>
+      <c r="K115" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
@@ -6374,13 +6313,15 @@
       <c r="G116" s="5">
         <v>1464</v>
       </c>
-      <c r="H116" s="58"/>
+      <c r="H116" s="43"/>
       <c r="I116" s="29" t="e">
-        <f>ВПР(A116;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J116"/>
-      <c r="K116" s="55"/>
+      <c r="K116" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
@@ -6404,13 +6345,15 @@
       <c r="G117" s="5">
         <v>1544</v>
       </c>
-      <c r="H117" s="58"/>
+      <c r="H117" s="43"/>
       <c r="I117" s="29" t="e">
-        <f>ВПР(A117;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J117"/>
-      <c r="K117" s="55"/>
+      <c r="K117" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
@@ -6434,13 +6377,15 @@
       <c r="G118" s="5">
         <v>1215</v>
       </c>
-      <c r="H118" s="58"/>
+      <c r="H118" s="43"/>
       <c r="I118" s="29" t="e">
-        <f>ВПР(A118;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J118"/>
-      <c r="K118" s="55"/>
+      <c r="K118" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
@@ -6464,13 +6409,15 @@
       <c r="G119" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H119" s="58"/>
+      <c r="H119" s="43"/>
       <c r="I119" s="29" t="e">
-        <f>ВПР(A119;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J119"/>
-      <c r="K119" s="55"/>
+      <c r="K119" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
@@ -6490,13 +6437,15 @@
       <c r="G120" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H120" s="58"/>
+      <c r="H120" s="43"/>
       <c r="I120" s="29" t="e">
-        <f>ВПР(A120;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J120"/>
-      <c r="K120" s="55"/>
+      <c r="K120" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
@@ -6512,13 +6461,15 @@
         <v>9</v>
       </c>
       <c r="G121" s="4"/>
-      <c r="H121" s="58"/>
+      <c r="H121" s="43"/>
       <c r="I121" s="29" t="e">
-        <f>ВПР(A121;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J121"/>
-      <c r="K121" s="55"/>
+      <c r="K121" s="40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
@@ -6542,13 +6493,15 @@
       <c r="G122" s="3">
         <v>1402</v>
       </c>
-      <c r="H122" s="58"/>
+      <c r="H122" s="43"/>
       <c r="I122" s="29" t="e">
-        <f>ВПР(A122;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J122"/>
-      <c r="K122" s="55"/>
+      <c r="K122" s="40">
+        <f t="shared" ref="K69:K125" si="2" xml:space="preserve"> SQRT(B122) * SQRT(E122) * IF(F122 &gt; 600, LOG(F122), SQRT(F122)) * SQRT(H122) / IF(F122 &gt; 600, 140, 1100) * IF(B122&lt;1300,  IF(B122&gt;1000, 1.4, 2 ), 1 )</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
@@ -6570,13 +6523,15 @@
       <c r="G123" s="3">
         <v>1400</v>
       </c>
-      <c r="H123" s="58"/>
+      <c r="H123" s="43"/>
       <c r="I123" s="29" t="e">
-        <f>ВПР(A123;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J123"/>
-      <c r="K123" s="55"/>
+      <c r="K123" s="40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
@@ -6600,13 +6555,15 @@
       <c r="G124" s="5">
         <v>1400</v>
       </c>
-      <c r="H124" s="58"/>
+      <c r="H124" s="43"/>
       <c r="I124" s="29" t="e">
-        <f>ВПР(A124;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J124"/>
-      <c r="K124" s="55"/>
+      <c r="K124" s="40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
@@ -6630,13 +6587,15 @@
       <c r="G125" s="5">
         <v>1620</v>
       </c>
-      <c r="H125" s="58"/>
+      <c r="H125" s="43"/>
       <c r="I125" s="29" t="e">
-        <f>ВПР(A125;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J125"/>
-      <c r="K125" s="55"/>
+      <c r="K125" s="40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
@@ -6660,13 +6619,15 @@
       <c r="G126" s="5">
         <v>1620</v>
       </c>
-      <c r="H126" s="58"/>
+      <c r="H126" s="43"/>
       <c r="I126" s="29" t="e">
-        <f>ВПР(A126;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J126"/>
-      <c r="K126" s="55"/>
+      <c r="K126" s="40" t="e">
+        <f t="shared" ref="K69:K127" si="3">SQRT(B126) * LOG(E126/100) * SQRT(LOG(F126)) * SQRT(H126)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
@@ -6690,13 +6651,15 @@
       <c r="G127" s="5">
         <v>1566</v>
       </c>
-      <c r="H127" s="58"/>
+      <c r="H127" s="43"/>
       <c r="I127" s="29" t="e">
-        <f>ВПР(A127;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J127"/>
-      <c r="K127" s="55"/>
+      <c r="K127" s="40" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
@@ -6720,13 +6683,15 @@
       <c r="G128" s="5">
         <v>1350</v>
       </c>
-      <c r="H128" s="58"/>
+      <c r="H128" s="43"/>
       <c r="I128" s="29" t="e">
-        <f>ВПР(A128;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J128"/>
-      <c r="K128" s="55"/>
+      <c r="K128" s="40" t="e">
+        <f t="shared" ref="K128:K130" si="4">LOG(B128) * SQRT(E128) * SQRT(LOG(F128)) * SQRT(H128) /7</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
@@ -6750,13 +6715,15 @@
       <c r="G129" s="5">
         <v>1300</v>
       </c>
-      <c r="H129" s="58"/>
+      <c r="H129" s="43"/>
       <c r="I129" s="29" t="e">
-        <f>ВПР(A129;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J129"/>
-      <c r="K129" s="55"/>
+      <c r="K129" s="40" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
@@ -6780,13 +6747,15 @@
       <c r="G130" s="5">
         <v>1215</v>
       </c>
-      <c r="H130" s="58"/>
+      <c r="H130" s="43"/>
       <c r="I130" s="29" t="e">
-        <f>ВПР(A130;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J130"/>
-      <c r="K130" s="55"/>
+      <c r="K130" s="40" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="131" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
@@ -6810,13 +6779,12 @@
       <c r="G131" s="5">
         <v>1215</v>
       </c>
-      <c r="H131" s="58"/>
+      <c r="H131" s="43"/>
       <c r="I131" s="29" t="e">
-        <f>ВПР(A131;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J131"/>
-      <c r="K131" s="55"/>
+      <c r="K131" s="40"/>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
@@ -6840,13 +6808,12 @@
       <c r="G132" s="5">
         <v>1401</v>
       </c>
-      <c r="H132" s="58"/>
+      <c r="H132" s="43"/>
       <c r="I132" s="29" t="e">
-        <f>ВПР(A132;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J132"/>
-      <c r="K132" s="55"/>
+      <c r="K132" s="40"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
@@ -6856,13 +6823,12 @@
       <c r="E133" s="27"/>
       <c r="F133" s="27"/>
       <c r="G133" s="5"/>
-      <c r="H133" s="58"/>
+      <c r="H133" s="43"/>
       <c r="I133" s="29" t="e">
-        <f>ВПР(A133;M:N;2;0)</f>
         <v>#N/A</v>
       </c>
       <c r="J133"/>
-      <c r="K133" s="55"/>
+      <c r="K133" s="40"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
@@ -6872,10 +6838,10 @@
       <c r="E134" s="24"/>
       <c r="F134" s="24"/>
       <c r="G134" s="4"/>
-      <c r="H134" s="58"/>
+      <c r="H134" s="43"/>
       <c r="I134" s="29"/>
       <c r="J134"/>
-      <c r="K134" s="55"/>
+      <c r="K134" s="40"/>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
@@ -6885,10 +6851,10 @@
       <c r="E135" s="24"/>
       <c r="F135" s="24"/>
       <c r="G135" s="4"/>
-      <c r="H135" s="58"/>
+      <c r="H135" s="43"/>
       <c r="I135" s="29"/>
       <c r="J135"/>
-      <c r="K135" s="55"/>
+      <c r="K135" s="40"/>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
@@ -6898,10 +6864,10 @@
       <c r="E136" s="24"/>
       <c r="F136" s="24"/>
       <c r="G136" s="4"/>
-      <c r="H136" s="58"/>
+      <c r="H136" s="43"/>
       <c r="I136" s="29"/>
       <c r="J136"/>
-      <c r="K136" s="55"/>
+      <c r="K136" s="40"/>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
@@ -6913,7 +6879,7 @@
       <c r="G137" s="3"/>
       <c r="I137" s="29"/>
       <c r="J137"/>
-      <c r="K137" s="55"/>
+      <c r="K137" s="40"/>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
@@ -6925,7 +6891,7 @@
       <c r="G138" s="3"/>
       <c r="I138" s="29"/>
       <c r="J138"/>
-      <c r="K138" s="55"/>
+      <c r="K138" s="40"/>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
@@ -6937,7 +6903,7 @@
       <c r="G139" s="3"/>
       <c r="I139" s="29"/>
       <c r="J139"/>
-      <c r="K139" s="55"/>
+      <c r="K139" s="40"/>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
@@ -6949,7 +6915,7 @@
       <c r="G140" s="3"/>
       <c r="I140" s="29"/>
       <c r="J140"/>
-      <c r="K140" s="55"/>
+      <c r="K140" s="40"/>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
@@ -6961,7 +6927,7 @@
       <c r="G141" s="3"/>
       <c r="I141" s="29"/>
       <c r="J141"/>
-      <c r="K141" s="55"/>
+      <c r="K141" s="40"/>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
@@ -6973,7 +6939,7 @@
       <c r="G142" s="3"/>
       <c r="I142" s="29"/>
       <c r="J142"/>
-      <c r="K142" s="55"/>
+      <c r="K142" s="40"/>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
@@ -6985,7 +6951,7 @@
       <c r="G143" s="5"/>
       <c r="I143" s="29"/>
       <c r="J143"/>
-      <c r="K143" s="55"/>
+      <c r="K143" s="40"/>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
@@ -6997,7 +6963,7 @@
       <c r="G144" s="4"/>
       <c r="I144" s="29"/>
       <c r="J144"/>
-      <c r="K144" s="55"/>
+      <c r="K144" s="40"/>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
@@ -7009,7 +6975,7 @@
       <c r="G145" s="4"/>
       <c r="I145" s="29"/>
       <c r="J145"/>
-      <c r="K145" s="55"/>
+      <c r="K145" s="40"/>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="4"/>
@@ -7021,7 +6987,7 @@
       <c r="G146" s="4"/>
       <c r="I146" s="29"/>
       <c r="J146"/>
-      <c r="K146" s="55"/>
+      <c r="K146" s="40"/>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
@@ -7033,7 +6999,7 @@
       <c r="G147" s="3"/>
       <c r="I147" s="29"/>
       <c r="J147"/>
-      <c r="K147" s="55"/>
+      <c r="K147" s="40"/>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
@@ -7045,7 +7011,7 @@
       <c r="G148" s="2"/>
       <c r="I148" s="29"/>
       <c r="J148"/>
-      <c r="K148" s="55"/>
+      <c r="K148" s="40"/>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
@@ -7057,7 +7023,7 @@
       <c r="G149" s="2"/>
       <c r="I149" s="29"/>
       <c r="J149"/>
-      <c r="K149" s="55"/>
+      <c r="K149" s="40"/>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
@@ -7069,7 +7035,7 @@
       <c r="G150" s="2"/>
       <c r="I150" s="29"/>
       <c r="J150"/>
-      <c r="K150" s="55"/>
+      <c r="K150" s="40"/>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>

</xml_diff>